<commit_message>
Undid Ai Shimizu Appearance patch
</commit_message>
<xml_diff>
--- a/TJPW Metrics.xlsx
+++ b/TJPW Metrics.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="520">
   <si>
     <t>`</t>
   </si>
@@ -1577,13 +1577,7 @@
     <t>Miyu Yamashita &amp; KANNA vs Yuka Sakazaki &amp; Ririko Kendo (Rika Tatsumi)</t>
   </si>
   <si>
-    <t>Ai Shimizu Appearance1</t>
-  </si>
-  <si>
-    <t>Ai Shimizu Appearance2</t>
-  </si>
-  <si>
-    <t>Ai Shimizu Appearance3</t>
+    <t>Ai Shimizu Appearance</t>
   </si>
 </sst>
 </file>
@@ -2137,56 +2131,68 @@
     <xf numFmtId="0" fontId="3" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2240,68 +2246,56 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2695,97 +2689,97 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="62" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="65" t="s">
+      <c r="G2" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="101"/>
+      <c r="I2" s="102" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="68" t="s">
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106"/>
+      <c r="Q2" s="107"/>
+      <c r="R2" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="71" t="s">
+      <c r="S2" s="109"/>
+      <c r="T2" s="109"/>
+      <c r="U2" s="109"/>
+      <c r="V2" s="110"/>
+      <c r="W2" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="72"/>
-      <c r="Z2" s="72"/>
-      <c r="AA2" s="72"/>
-      <c r="AB2" s="72"/>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="72"/>
-      <c r="AE2" s="72"/>
-      <c r="AF2" s="73"/>
-      <c r="AG2" s="74" t="s">
+      <c r="X2" s="112"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="112"/>
+      <c r="AA2" s="112"/>
+      <c r="AB2" s="112"/>
+      <c r="AC2" s="112"/>
+      <c r="AD2" s="112"/>
+      <c r="AE2" s="112"/>
+      <c r="AF2" s="113"/>
+      <c r="AG2" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="AH2" s="75"/>
-      <c r="AI2" s="75"/>
-      <c r="AJ2" s="75"/>
-      <c r="AK2" s="75"/>
-      <c r="AL2" s="75"/>
-      <c r="AM2" s="75"/>
-      <c r="AN2" s="76"/>
-      <c r="AO2" s="77" t="s">
+      <c r="AH2" s="115"/>
+      <c r="AI2" s="115"/>
+      <c r="AJ2" s="115"/>
+      <c r="AK2" s="115"/>
+      <c r="AL2" s="115"/>
+      <c r="AM2" s="115"/>
+      <c r="AN2" s="116"/>
+      <c r="AO2" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="AP2" s="78"/>
-      <c r="AQ2" s="78"/>
-      <c r="AR2" s="78"/>
-      <c r="AS2" s="78"/>
-      <c r="AT2" s="79"/>
-      <c r="AU2" s="80" t="s">
+      <c r="AP2" s="84"/>
+      <c r="AQ2" s="84"/>
+      <c r="AR2" s="84"/>
+      <c r="AS2" s="84"/>
+      <c r="AT2" s="85"/>
+      <c r="AU2" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="AV2" s="81"/>
-      <c r="AW2" s="82" t="s">
+      <c r="AV2" s="87"/>
+      <c r="AW2" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="AX2" s="83"/>
-      <c r="AY2" s="83"/>
-      <c r="AZ2" s="83"/>
-      <c r="BA2" s="83"/>
-      <c r="BB2" s="83"/>
-      <c r="BC2" s="83"/>
-      <c r="BD2" s="84"/>
-      <c r="BE2" s="85" t="s">
+      <c r="AX2" s="89"/>
+      <c r="AY2" s="89"/>
+      <c r="AZ2" s="89"/>
+      <c r="BA2" s="89"/>
+      <c r="BB2" s="89"/>
+      <c r="BC2" s="89"/>
+      <c r="BD2" s="90"/>
+      <c r="BE2" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="BF2" s="86"/>
-      <c r="BG2" s="86"/>
-      <c r="BH2" s="87"/>
+      <c r="BF2" s="92"/>
+      <c r="BG2" s="92"/>
+      <c r="BH2" s="93"/>
       <c r="BI2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="BJ2" s="88" t="s">
+      <c r="BJ2" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="BK2" s="89"/>
-      <c r="BL2" s="90"/>
-      <c r="BM2" s="91" t="s">
+      <c r="BK2" s="95"/>
+      <c r="BL2" s="96"/>
+      <c r="BM2" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="BN2" s="92"/>
-      <c r="BO2" s="92"/>
-      <c r="BP2" s="92"/>
-      <c r="BQ2" s="92"/>
-      <c r="BR2" s="92"/>
-      <c r="BS2" s="93"/>
+      <c r="BN2" s="98"/>
+      <c r="BO2" s="98"/>
+      <c r="BP2" s="98"/>
+      <c r="BQ2" s="98"/>
+      <c r="BR2" s="98"/>
+      <c r="BS2" s="99"/>
     </row>
     <row r="3" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
@@ -2806,18 +2800,18 @@
       <c r="F3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="94">
+      <c r="G3" s="76">
         <v>2020</v>
       </c>
-      <c r="H3" s="95"/>
-      <c r="I3" s="96" t="s">
+      <c r="H3" s="77"/>
+      <c r="I3" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="97"/>
-      <c r="K3" s="98" t="s">
+      <c r="J3" s="79"/>
+      <c r="K3" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="96"/>
+      <c r="L3" s="78"/>
       <c r="M3" s="14" t="s">
         <v>21</v>
       </c>
@@ -2848,74 +2842,74 @@
       <c r="V3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="99" t="s">
+      <c r="W3" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="100"/>
-      <c r="Y3" s="99" t="s">
+      <c r="X3" s="82"/>
+      <c r="Y3" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="Z3" s="101"/>
-      <c r="AA3" s="101" t="s">
+      <c r="Z3" s="72"/>
+      <c r="AA3" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="101"/>
-      <c r="AC3" s="101" t="s">
+      <c r="AB3" s="72"/>
+      <c r="AC3" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="AD3" s="101"/>
-      <c r="AE3" s="101" t="s">
+      <c r="AD3" s="72"/>
+      <c r="AE3" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="AF3" s="101"/>
-      <c r="AG3" s="102" t="s">
+      <c r="AF3" s="72"/>
+      <c r="AG3" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="103"/>
-      <c r="AI3" s="104" t="s">
+      <c r="AH3" s="74"/>
+      <c r="AI3" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="AJ3" s="102"/>
-      <c r="AK3" s="102" t="s">
+      <c r="AJ3" s="73"/>
+      <c r="AK3" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="AL3" s="102"/>
-      <c r="AM3" s="102" t="s">
+      <c r="AL3" s="73"/>
+      <c r="AM3" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="AN3" s="103"/>
-      <c r="AO3" s="105" t="s">
+      <c r="AN3" s="74"/>
+      <c r="AO3" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="AP3" s="106"/>
-      <c r="AQ3" s="105" t="s">
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="AR3" s="107"/>
-      <c r="AS3" s="107" t="s">
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="AT3" s="106"/>
-      <c r="AU3" s="108" t="s">
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="AV3" s="109"/>
-      <c r="AW3" s="110" t="s">
+      <c r="AV3" s="70"/>
+      <c r="AW3" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="AX3" s="111"/>
-      <c r="AY3" s="111" t="s">
+      <c r="AX3" s="63"/>
+      <c r="AY3" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="AZ3" s="111"/>
-      <c r="BA3" s="111" t="s">
+      <c r="AZ3" s="63"/>
+      <c r="BA3" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="BB3" s="111"/>
-      <c r="BC3" s="112" t="s">
+      <c r="BB3" s="63"/>
+      <c r="BC3" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="BD3" s="113"/>
+      <c r="BD3" s="65"/>
       <c r="BE3" s="22" t="s">
         <v>19</v>
       </c>
@@ -11806,6 +11800,30 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="BM2:BS2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="W2:AF2"/>
+    <mergeCell ref="AG2:AN2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AW2:BD2"/>
+    <mergeCell ref="BE2:BH2"/>
+    <mergeCell ref="BJ2:BL2"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="AK3:AL3"/>
     <mergeCell ref="BA3:BB3"/>
     <mergeCell ref="BC3:BD3"/>
     <mergeCell ref="AO3:AP3"/>
@@ -11814,30 +11832,6 @@
     <mergeCell ref="AU3:AV3"/>
     <mergeCell ref="AW3:AX3"/>
     <mergeCell ref="AY3:AZ3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AW2:BD2"/>
-    <mergeCell ref="BE2:BH2"/>
-    <mergeCell ref="BJ2:BL2"/>
-    <mergeCell ref="BM2:BS2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="W2:AF2"/>
-    <mergeCell ref="AG2:AN2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11941,7 +11935,7 @@
       <c r="A2" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="115">
+      <c r="B2" s="61">
         <v>41304</v>
       </c>
       <c r="C2" t="s">
@@ -11953,10 +11947,10 @@
       <c r="E2" t="s">
         <v>152</v>
       </c>
-      <c r="F2" s="116" t="s">
+      <c r="F2" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="G2" s="114" t="s">
+      <c r="G2" s="60" t="s">
         <v>149</v>
       </c>
       <c r="H2" t="s">
@@ -11976,7 +11970,7 @@
       <c r="A3" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="115">
+      <c r="B3" s="61">
         <v>41358</v>
       </c>
       <c r="C3" t="s">
@@ -11988,7 +11982,7 @@
       <c r="E3" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="116" t="s">
+      <c r="F3" s="62" t="s">
         <v>268</v>
       </c>
       <c r="G3" t="s">
@@ -12011,7 +12005,7 @@
       <c r="A4" t="s">
         <v>153</v>
       </c>
-      <c r="B4" s="115">
+      <c r="B4" s="61">
         <v>41390</v>
       </c>
       <c r="C4" t="s">
@@ -12023,7 +12017,7 @@
       <c r="E4" t="s">
         <v>154</v>
       </c>
-      <c r="F4" s="116" t="s">
+      <c r="F4" s="62" t="s">
         <v>269</v>
       </c>
       <c r="G4" t="s">
@@ -12046,7 +12040,7 @@
       <c r="A5" t="s">
         <v>157</v>
       </c>
-      <c r="B5" s="115">
+      <c r="B5" s="61">
         <v>41431</v>
       </c>
       <c r="C5" t="s">
@@ -12058,7 +12052,7 @@
       <c r="E5" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="116" t="s">
+      <c r="F5" s="62" t="s">
         <v>270</v>
       </c>
       <c r="G5" t="s">
@@ -12081,7 +12075,7 @@
       <c r="A6" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="115">
+      <c r="B6" s="61">
         <v>41431</v>
       </c>
       <c r="C6" t="s">
@@ -12093,7 +12087,7 @@
       <c r="E6" t="s">
         <v>161</v>
       </c>
-      <c r="F6" s="116" t="s">
+      <c r="F6" s="62" t="s">
         <v>271</v>
       </c>
       <c r="G6" t="s">
@@ -12116,7 +12110,7 @@
       <c r="A7" t="s">
         <v>162</v>
       </c>
-      <c r="B7" s="115">
+      <c r="B7" s="61">
         <v>41466</v>
       </c>
       <c r="C7" t="s">
@@ -12128,7 +12122,7 @@
       <c r="E7" t="s">
         <v>163</v>
       </c>
-      <c r="F7" s="116" t="s">
+      <c r="F7" s="62" t="s">
         <v>272</v>
       </c>
       <c r="G7" t="s">
@@ -12151,7 +12145,7 @@
       <c r="A8" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="115">
+      <c r="B8" s="61">
         <v>41466</v>
       </c>
       <c r="C8" t="s">
@@ -12163,7 +12157,7 @@
       <c r="E8" t="s">
         <v>154</v>
       </c>
-      <c r="F8" s="116" t="s">
+      <c r="F8" s="62" t="s">
         <v>273</v>
       </c>
       <c r="G8" t="s">
@@ -12186,7 +12180,7 @@
       <c r="A9" t="s">
         <v>164</v>
       </c>
-      <c r="B9" s="115">
+      <c r="B9" s="61">
         <v>41565</v>
       </c>
       <c r="C9" t="s">
@@ -12198,7 +12192,7 @@
       <c r="E9" t="s">
         <v>165</v>
       </c>
-      <c r="F9" s="116" t="s">
+      <c r="F9" s="62" t="s">
         <v>274</v>
       </c>
       <c r="G9" t="s">
@@ -12221,7 +12215,7 @@
       <c r="A10" t="s">
         <v>164</v>
       </c>
-      <c r="B10" s="115">
+      <c r="B10" s="61">
         <v>41565</v>
       </c>
       <c r="C10" t="s">
@@ -12233,7 +12227,7 @@
       <c r="E10" t="s">
         <v>152</v>
       </c>
-      <c r="F10" s="116" t="s">
+      <c r="F10" s="62" t="s">
         <v>275</v>
       </c>
       <c r="G10" t="s">
@@ -12256,7 +12250,7 @@
       <c r="A11" t="s">
         <v>167</v>
       </c>
-      <c r="B11" s="115">
+      <c r="B11" s="61">
         <v>41609</v>
       </c>
       <c r="C11" t="s">
@@ -12268,7 +12262,7 @@
       <c r="E11" t="s">
         <v>168</v>
       </c>
-      <c r="F11" s="116" t="s">
+      <c r="F11" s="62" t="s">
         <v>276</v>
       </c>
       <c r="G11" t="s">
@@ -12291,7 +12285,7 @@
       <c r="A12" t="s">
         <v>167</v>
       </c>
-      <c r="B12" s="115">
+      <c r="B12" s="61">
         <v>41609</v>
       </c>
       <c r="C12" t="s">
@@ -12303,7 +12297,7 @@
       <c r="E12" t="s">
         <v>169</v>
       </c>
-      <c r="F12" s="116" t="s">
+      <c r="F12" s="62" t="s">
         <v>277</v>
       </c>
       <c r="G12" t="s">
@@ -12338,7 +12332,7 @@
       <c r="A13" t="s">
         <v>167</v>
       </c>
-      <c r="B13" s="115">
+      <c r="B13" s="61">
         <v>41609</v>
       </c>
       <c r="C13" t="s">
@@ -12350,7 +12344,7 @@
       <c r="E13" t="s">
         <v>161</v>
       </c>
-      <c r="F13" s="116" t="s">
+      <c r="F13" s="62" t="s">
         <v>278</v>
       </c>
       <c r="G13" t="s">
@@ -12370,43 +12364,43 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F14" s="116"/>
+      <c r="F14" s="62"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F15" s="116"/>
+      <c r="F15" s="62"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="F16" s="116"/>
+      <c r="F16" s="62"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="116"/>
+      <c r="F17" s="62"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="116"/>
+      <c r="F18" s="62"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="116"/>
+      <c r="F19" s="62"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="116"/>
+      <c r="F20" s="62"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="116"/>
+      <c r="F21" s="62"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="116"/>
+      <c r="F22" s="62"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="116"/>
+      <c r="F23" s="62"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="116"/>
+      <c r="F24" s="62"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="116"/>
+      <c r="F25" s="62"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="116"/>
+      <c r="F26" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12417,8 +12411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12511,7 +12505,7 @@
       <c r="A2" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="115">
+      <c r="B2" s="61">
         <v>41657</v>
       </c>
       <c r="C2" t="s">
@@ -12523,10 +12517,10 @@
       <c r="E2" t="s">
         <v>177</v>
       </c>
-      <c r="F2" s="114" t="s">
+      <c r="F2" s="60" t="s">
         <v>279</v>
       </c>
-      <c r="G2" s="114" t="s">
+      <c r="G2" s="60" t="s">
         <v>149</v>
       </c>
       <c r="H2" t="s">
@@ -12546,7 +12540,7 @@
       <c r="A3" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="115">
+      <c r="B3" s="61">
         <v>41657</v>
       </c>
       <c r="C3" t="s">
@@ -12558,7 +12552,7 @@
       <c r="E3" t="s">
         <v>178</v>
       </c>
-      <c r="F3" s="114" t="s">
+      <c r="F3" s="60" t="s">
         <v>280</v>
       </c>
       <c r="G3" t="s">
@@ -12581,7 +12575,7 @@
       <c r="A4" t="s">
         <v>176</v>
       </c>
-      <c r="B4" s="115">
+      <c r="B4" s="61">
         <v>41657</v>
       </c>
       <c r="C4" t="s">
@@ -12593,7 +12587,7 @@
       <c r="E4" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="114" t="s">
+      <c r="F4" s="60" t="s">
         <v>281</v>
       </c>
       <c r="G4" t="s">
@@ -12616,7 +12610,7 @@
       <c r="A5" t="s">
         <v>180</v>
       </c>
-      <c r="B5" s="115">
+      <c r="B5" s="61">
         <v>41667</v>
       </c>
       <c r="C5" t="s">
@@ -12628,7 +12622,7 @@
       <c r="E5" t="s">
         <v>513</v>
       </c>
-      <c r="F5" s="114" t="s">
+      <c r="F5" s="60" t="s">
         <v>282</v>
       </c>
       <c r="G5" t="s">
@@ -12651,7 +12645,7 @@
       <c r="A6" t="s">
         <v>180</v>
       </c>
-      <c r="B6" s="115">
+      <c r="B6" s="61">
         <v>41667</v>
       </c>
       <c r="C6" t="s">
@@ -12663,7 +12657,7 @@
       <c r="E6" t="s">
         <v>183</v>
       </c>
-      <c r="F6" s="114" t="s">
+      <c r="F6" s="60" t="s">
         <v>283</v>
       </c>
       <c r="G6" t="s">
@@ -12686,7 +12680,7 @@
       <c r="A7" t="s">
         <v>180</v>
       </c>
-      <c r="B7" s="115">
+      <c r="B7" s="61">
         <v>41667</v>
       </c>
       <c r="C7" t="s">
@@ -12698,7 +12692,7 @@
       <c r="E7" t="s">
         <v>184</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="60" t="s">
         <v>284</v>
       </c>
       <c r="G7" t="s">
@@ -12721,7 +12715,7 @@
       <c r="A8" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="115">
+      <c r="B8" s="61">
         <v>41685</v>
       </c>
       <c r="C8" t="s">
@@ -12733,7 +12727,7 @@
       <c r="E8" t="s">
         <v>187</v>
       </c>
-      <c r="F8" s="114" t="s">
+      <c r="F8" s="60" t="s">
         <v>285</v>
       </c>
       <c r="G8" t="s">
@@ -12756,7 +12750,7 @@
       <c r="A9" t="s">
         <v>185</v>
       </c>
-      <c r="B9" s="115">
+      <c r="B9" s="61">
         <v>41685</v>
       </c>
       <c r="C9" t="s">
@@ -12768,7 +12762,7 @@
       <c r="E9" t="s">
         <v>512</v>
       </c>
-      <c r="F9" s="114" t="s">
+      <c r="F9" s="60" t="s">
         <v>286</v>
       </c>
       <c r="G9" t="s">
@@ -12791,7 +12785,7 @@
       <c r="A10" t="s">
         <v>185</v>
       </c>
-      <c r="B10" s="115">
+      <c r="B10" s="61">
         <v>41685</v>
       </c>
       <c r="C10" t="s">
@@ -12803,7 +12797,7 @@
       <c r="E10" t="s">
         <v>188</v>
       </c>
-      <c r="F10" s="114" t="s">
+      <c r="F10" s="60" t="s">
         <v>287</v>
       </c>
       <c r="G10" t="s">
@@ -12838,7 +12832,7 @@
       <c r="A11" t="s">
         <v>189</v>
       </c>
-      <c r="B11" s="115">
+      <c r="B11" s="61">
         <v>41697</v>
       </c>
       <c r="C11" t="s">
@@ -12850,7 +12844,7 @@
       <c r="E11" t="s">
         <v>154</v>
       </c>
-      <c r="F11" s="114" t="s">
+      <c r="F11" s="60" t="s">
         <v>288</v>
       </c>
       <c r="G11" t="s">
@@ -12873,7 +12867,7 @@
       <c r="A12" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="115">
+      <c r="B12" s="61">
         <v>41697</v>
       </c>
       <c r="C12" t="s">
@@ -12885,7 +12879,7 @@
       <c r="E12" t="s">
         <v>514</v>
       </c>
-      <c r="F12" s="114" t="s">
+      <c r="F12" s="60" t="s">
         <v>282</v>
       </c>
       <c r="G12" t="s">
@@ -12914,7 +12908,7 @@
       <c r="A13" t="s">
         <v>189</v>
       </c>
-      <c r="B13" s="115">
+      <c r="B13" s="61">
         <v>41697</v>
       </c>
       <c r="C13" t="s">
@@ -12926,7 +12920,7 @@
       <c r="E13" t="s">
         <v>184</v>
       </c>
-      <c r="F13" s="114" t="s">
+      <c r="F13" s="60" t="s">
         <v>289</v>
       </c>
       <c r="G13" t="s">
@@ -12949,7 +12943,7 @@
       <c r="A14" t="s">
         <v>191</v>
       </c>
-      <c r="B14" s="115">
+      <c r="B14" s="61">
         <v>41713</v>
       </c>
       <c r="C14" t="s">
@@ -12961,7 +12955,7 @@
       <c r="E14" t="s">
         <v>212</v>
       </c>
-      <c r="F14" s="114" t="s">
+      <c r="F14" s="60" t="s">
         <v>290</v>
       </c>
       <c r="G14" t="s">
@@ -12987,7 +12981,7 @@
       <c r="A15" t="s">
         <v>191</v>
       </c>
-      <c r="B15" s="115">
+      <c r="B15" s="61">
         <v>41713</v>
       </c>
       <c r="C15" t="s">
@@ -12999,7 +12993,7 @@
       <c r="E15" t="s">
         <v>212</v>
       </c>
-      <c r="F15" s="114" t="s">
+      <c r="F15" s="60" t="s">
         <v>291</v>
       </c>
       <c r="G15" t="s">
@@ -13025,7 +13019,7 @@
       <c r="A16" t="s">
         <v>191</v>
       </c>
-      <c r="B16" s="115">
+      <c r="B16" s="61">
         <v>41713</v>
       </c>
       <c r="C16" t="s">
@@ -13037,7 +13031,7 @@
       <c r="E16" t="s">
         <v>192</v>
       </c>
-      <c r="F16" s="114" t="s">
+      <c r="F16" s="60" t="s">
         <v>292</v>
       </c>
       <c r="G16" t="s">
@@ -13060,7 +13054,7 @@
       <c r="A17" t="s">
         <v>191</v>
       </c>
-      <c r="B17" s="115">
+      <c r="B17" s="61">
         <v>41713</v>
       </c>
       <c r="C17" t="s">
@@ -13072,7 +13066,7 @@
       <c r="E17" t="s">
         <v>515</v>
       </c>
-      <c r="F17" s="114" t="s">
+      <c r="F17" s="60" t="s">
         <v>287</v>
       </c>
       <c r="G17" t="s">
@@ -13107,7 +13101,7 @@
       <c r="A18" t="s">
         <v>193</v>
       </c>
-      <c r="B18" s="115">
+      <c r="B18" s="61">
         <v>41734</v>
       </c>
       <c r="C18" t="s">
@@ -13119,7 +13113,7 @@
       <c r="E18" t="s">
         <v>195</v>
       </c>
-      <c r="F18" s="114" t="s">
+      <c r="F18" s="60" t="s">
         <v>293</v>
       </c>
       <c r="G18" t="s">
@@ -13142,7 +13136,7 @@
       <c r="A19" t="s">
         <v>193</v>
       </c>
-      <c r="B19" s="115">
+      <c r="B19" s="61">
         <v>41734</v>
       </c>
       <c r="C19" t="s">
@@ -13154,7 +13148,7 @@
       <c r="E19" t="s">
         <v>516</v>
       </c>
-      <c r="F19" s="114" t="s">
+      <c r="F19" s="60" t="s">
         <v>294</v>
       </c>
       <c r="G19" t="s">
@@ -13183,7 +13177,7 @@
       <c r="A20" t="s">
         <v>193</v>
       </c>
-      <c r="B20" s="115">
+      <c r="B20" s="61">
         <v>41734</v>
       </c>
       <c r="C20" t="s">
@@ -13195,7 +13189,7 @@
       <c r="E20" t="s">
         <v>196</v>
       </c>
-      <c r="F20" s="114" t="s">
+      <c r="F20" s="60" t="s">
         <v>295</v>
       </c>
       <c r="G20" t="s">
@@ -13218,7 +13212,7 @@
       <c r="A21" t="s">
         <v>193</v>
       </c>
-      <c r="B21" s="115">
+      <c r="B21" s="61">
         <v>41734</v>
       </c>
       <c r="C21" t="s">
@@ -13230,7 +13224,7 @@
       <c r="E21" t="s">
         <v>197</v>
       </c>
-      <c r="F21" s="114" t="s">
+      <c r="F21" s="60" t="s">
         <v>296</v>
       </c>
       <c r="G21" t="s">
@@ -13253,7 +13247,7 @@
       <c r="A22" t="s">
         <v>201</v>
       </c>
-      <c r="B22" s="115">
+      <c r="B22" s="61">
         <v>41755</v>
       </c>
       <c r="C22" t="s">
@@ -13265,7 +13259,7 @@
       <c r="E22" t="s">
         <v>202</v>
       </c>
-      <c r="F22" s="114" t="s">
+      <c r="F22" s="60" t="s">
         <v>297</v>
       </c>
       <c r="G22" t="s">
@@ -13288,7 +13282,7 @@
       <c r="A23" t="s">
         <v>201</v>
       </c>
-      <c r="B23" s="115">
+      <c r="B23" s="61">
         <v>41755</v>
       </c>
       <c r="C23" t="s">
@@ -13300,7 +13294,7 @@
       <c r="E23" t="s">
         <v>517</v>
       </c>
-      <c r="F23" s="114" t="s">
+      <c r="F23" s="60" t="s">
         <v>298</v>
       </c>
       <c r="G23" t="s">
@@ -13323,7 +13317,7 @@
       <c r="A24" t="s">
         <v>201</v>
       </c>
-      <c r="B24" s="115">
+      <c r="B24" s="61">
         <v>41755</v>
       </c>
       <c r="C24" t="s">
@@ -13335,7 +13329,7 @@
       <c r="E24" t="s">
         <v>203</v>
       </c>
-      <c r="F24" s="114" t="s">
+      <c r="F24" s="60" t="s">
         <v>299</v>
       </c>
       <c r="G24" t="s">
@@ -13370,7 +13364,7 @@
       <c r="A25" t="s">
         <v>204</v>
       </c>
-      <c r="B25" s="115">
+      <c r="B25" s="61">
         <v>41783</v>
       </c>
       <c r="C25" t="s">
@@ -13382,7 +13376,7 @@
       <c r="E25" t="s">
         <v>205</v>
       </c>
-      <c r="F25" s="114" t="s">
+      <c r="F25" s="60" t="s">
         <v>300</v>
       </c>
       <c r="G25" t="s">
@@ -13405,7 +13399,7 @@
       <c r="A26" t="s">
         <v>204</v>
       </c>
-      <c r="B26" s="115">
+      <c r="B26" s="61">
         <v>41783</v>
       </c>
       <c r="C26" t="s">
@@ -13417,7 +13411,7 @@
       <c r="E26" t="s">
         <v>518</v>
       </c>
-      <c r="F26" s="114" t="s">
+      <c r="F26" s="60" t="s">
         <v>301</v>
       </c>
       <c r="G26" t="s">
@@ -13452,7 +13446,7 @@
       <c r="A27" t="s">
         <v>204</v>
       </c>
-      <c r="B27" s="115">
+      <c r="B27" s="61">
         <v>41783</v>
       </c>
       <c r="C27" t="s">
@@ -13464,7 +13458,7 @@
       <c r="E27" t="s">
         <v>206</v>
       </c>
-      <c r="F27" s="114" t="s">
+      <c r="F27" s="60" t="s">
         <v>302</v>
       </c>
       <c r="G27" t="s">
@@ -13487,7 +13481,7 @@
       <c r="A28" t="s">
         <v>213</v>
       </c>
-      <c r="B28" s="115">
+      <c r="B28" s="61">
         <v>41794</v>
       </c>
       <c r="C28" t="s">
@@ -13499,7 +13493,7 @@
       <c r="E28" t="s">
         <v>214</v>
       </c>
-      <c r="F28" s="114" t="s">
+      <c r="F28" s="60" t="s">
         <v>303</v>
       </c>
       <c r="G28" t="s">
@@ -13525,7 +13519,7 @@
       <c r="A29" t="s">
         <v>213</v>
       </c>
-      <c r="B29" s="115">
+      <c r="B29" s="61">
         <v>41794</v>
       </c>
       <c r="C29" t="s">
@@ -13537,7 +13531,7 @@
       <c r="E29" t="s">
         <v>215</v>
       </c>
-      <c r="F29" s="114" t="s">
+      <c r="F29" s="60" t="s">
         <v>290</v>
       </c>
       <c r="G29" t="s">
@@ -13563,7 +13557,7 @@
       <c r="A30" t="s">
         <v>213</v>
       </c>
-      <c r="B30" s="115">
+      <c r="B30" s="61">
         <v>41794</v>
       </c>
       <c r="C30" t="s">
@@ -13575,7 +13569,7 @@
       <c r="E30" t="s">
         <v>202</v>
       </c>
-      <c r="F30" s="114" t="s">
+      <c r="F30" s="60" t="s">
         <v>290</v>
       </c>
       <c r="G30" t="s">
@@ -13601,7 +13595,7 @@
       <c r="A31" t="s">
         <v>213</v>
       </c>
-      <c r="B31" s="115">
+      <c r="B31" s="61">
         <v>41794</v>
       </c>
       <c r="C31" t="s">
@@ -13613,7 +13607,7 @@
       <c r="E31" t="s">
         <v>206</v>
       </c>
-      <c r="F31" s="114" t="s">
+      <c r="F31" s="60" t="s">
         <v>304</v>
       </c>
       <c r="G31" t="s">
@@ -13636,7 +13630,7 @@
       <c r="A32" t="s">
         <v>207</v>
       </c>
-      <c r="B32" s="115">
+      <c r="B32" s="61">
         <v>41812</v>
       </c>
       <c r="C32" t="s">
@@ -13648,7 +13642,7 @@
       <c r="E32" t="s">
         <v>208</v>
       </c>
-      <c r="F32" s="114" t="s">
+      <c r="F32" s="60" t="s">
         <v>305</v>
       </c>
       <c r="G32" t="s">
@@ -13677,7 +13671,7 @@
       <c r="A33" t="s">
         <v>207</v>
       </c>
-      <c r="B33" s="115">
+      <c r="B33" s="61">
         <v>41812</v>
       </c>
       <c r="C33" t="s">
@@ -13689,7 +13683,7 @@
       <c r="E33" t="s">
         <v>209</v>
       </c>
-      <c r="F33" s="114" t="s">
+      <c r="F33" s="60" t="s">
         <v>306</v>
       </c>
       <c r="G33" t="s">
@@ -13715,7 +13709,7 @@
       <c r="A34" t="s">
         <v>207</v>
       </c>
-      <c r="B34" s="115">
+      <c r="B34" s="61">
         <v>41812</v>
       </c>
       <c r="C34" t="s">
@@ -13727,7 +13721,7 @@
       <c r="E34" t="s">
         <v>202</v>
       </c>
-      <c r="F34" s="114" t="s">
+      <c r="F34" s="60" t="s">
         <v>307</v>
       </c>
       <c r="G34" t="s">
@@ -13753,7 +13747,7 @@
       <c r="A35" t="s">
         <v>217</v>
       </c>
-      <c r="B35" s="115">
+      <c r="B35" s="61">
         <v>41831</v>
       </c>
       <c r="C35" t="s">
@@ -13765,7 +13759,7 @@
       <c r="E35" t="s">
         <v>219</v>
       </c>
-      <c r="F35" s="114" t="s">
+      <c r="F35" s="60" t="s">
         <v>308</v>
       </c>
       <c r="G35" t="s">
@@ -13791,7 +13785,7 @@
       <c r="A36" t="s">
         <v>217</v>
       </c>
-      <c r="B36" s="115">
+      <c r="B36" s="61">
         <v>41831</v>
       </c>
       <c r="C36" t="s">
@@ -13803,7 +13797,7 @@
       <c r="E36" t="s">
         <v>220</v>
       </c>
-      <c r="F36" s="114" t="s">
+      <c r="F36" s="60" t="s">
         <v>309</v>
       </c>
       <c r="G36" t="s">
@@ -13826,7 +13820,7 @@
       <c r="A37" t="s">
         <v>217</v>
       </c>
-      <c r="B37" s="115">
+      <c r="B37" s="61">
         <v>41831</v>
       </c>
       <c r="C37" t="s">
@@ -13838,7 +13832,7 @@
       <c r="E37" t="s">
         <v>221</v>
       </c>
-      <c r="F37" s="114" t="s">
+      <c r="F37" s="60" t="s">
         <v>310</v>
       </c>
       <c r="G37" t="s">
@@ -13873,7 +13867,7 @@
       <c r="A38" t="s">
         <v>222</v>
       </c>
-      <c r="B38" s="115">
+      <c r="B38" s="61">
         <v>41839</v>
       </c>
       <c r="C38" t="s">
@@ -13885,7 +13879,7 @@
       <c r="E38" t="s">
         <v>224</v>
       </c>
-      <c r="F38" s="114" t="s">
+      <c r="F38" s="60" t="s">
         <v>311</v>
       </c>
       <c r="G38" t="s">
@@ -13920,7 +13914,7 @@
       <c r="A39" t="s">
         <v>222</v>
       </c>
-      <c r="B39" s="115">
+      <c r="B39" s="61">
         <v>41839</v>
       </c>
       <c r="C39" t="s">
@@ -13932,7 +13926,7 @@
       <c r="E39" t="s">
         <v>225</v>
       </c>
-      <c r="F39" s="114" t="s">
+      <c r="F39" s="60" t="s">
         <v>312</v>
       </c>
       <c r="G39" t="s">
@@ -13958,7 +13952,7 @@
       <c r="A40" t="s">
         <v>222</v>
       </c>
-      <c r="B40" s="115">
+      <c r="B40" s="61">
         <v>41839</v>
       </c>
       <c r="C40" t="s">
@@ -13970,7 +13964,7 @@
       <c r="E40" t="s">
         <v>226</v>
       </c>
-      <c r="F40" s="114" t="s">
+      <c r="F40" s="60" t="s">
         <v>313</v>
       </c>
       <c r="G40" t="s">
@@ -13996,7 +13990,7 @@
       <c r="A41" t="s">
         <v>228</v>
       </c>
-      <c r="B41" s="115">
+      <c r="B41" s="61">
         <v>41853</v>
       </c>
       <c r="C41" t="s">
@@ -14008,7 +14002,7 @@
       <c r="E41" t="s">
         <v>230</v>
       </c>
-      <c r="F41" s="114" t="s">
+      <c r="F41" s="60" t="s">
         <v>314</v>
       </c>
       <c r="G41" t="s">
@@ -14037,7 +14031,7 @@
       <c r="A42" t="s">
         <v>228</v>
       </c>
-      <c r="B42" s="115">
+      <c r="B42" s="61">
         <v>41853</v>
       </c>
       <c r="C42" t="s">
@@ -14049,7 +14043,7 @@
       <c r="E42" t="s">
         <v>231</v>
       </c>
-      <c r="F42" s="114" t="s">
+      <c r="F42" s="60" t="s">
         <v>315</v>
       </c>
       <c r="G42" t="s">
@@ -14075,7 +14069,7 @@
       <c r="A43" t="s">
         <v>228</v>
       </c>
-      <c r="B43" s="115">
+      <c r="B43" s="61">
         <v>41853</v>
       </c>
       <c r="C43" t="s">
@@ -14087,7 +14081,7 @@
       <c r="E43" t="s">
         <v>178</v>
       </c>
-      <c r="F43" s="114" t="s">
+      <c r="F43" s="60" t="s">
         <v>316</v>
       </c>
       <c r="G43" t="s">
@@ -14113,7 +14107,7 @@
       <c r="A44" t="s">
         <v>228</v>
       </c>
-      <c r="B44" s="115">
+      <c r="B44" s="61">
         <v>41853</v>
       </c>
       <c r="C44" t="s">
@@ -14125,7 +14119,7 @@
       <c r="E44" t="s">
         <v>154</v>
       </c>
-      <c r="F44" s="114" t="s">
+      <c r="F44" s="60" t="s">
         <v>317</v>
       </c>
       <c r="G44" t="s">
@@ -14148,7 +14142,7 @@
       <c r="A45" t="s">
         <v>228</v>
       </c>
-      <c r="B45" s="115">
+      <c r="B45" s="61">
         <v>41853</v>
       </c>
       <c r="C45" t="s">
@@ -14160,7 +14154,7 @@
       <c r="E45" t="s">
         <v>232</v>
       </c>
-      <c r="F45" s="114" t="s">
+      <c r="F45" s="60" t="s">
         <v>318</v>
       </c>
       <c r="G45" t="s">
@@ -14186,7 +14180,7 @@
       <c r="A46" t="s">
         <v>235</v>
       </c>
-      <c r="B46" s="115">
+      <c r="B46" s="61">
         <v>41881</v>
       </c>
       <c r="C46" t="s">
@@ -14198,7 +14192,7 @@
       <c r="E46" t="s">
         <v>236</v>
       </c>
-      <c r="F46" s="114" t="s">
+      <c r="F46" s="60" t="s">
         <v>319</v>
       </c>
       <c r="G46" t="s">
@@ -14221,7 +14215,7 @@
       <c r="A47" t="s">
         <v>235</v>
       </c>
-      <c r="B47" s="115">
+      <c r="B47" s="61">
         <v>41881</v>
       </c>
       <c r="C47" t="s">
@@ -14233,7 +14227,7 @@
       <c r="E47" t="s">
         <v>237</v>
       </c>
-      <c r="F47" s="114" t="s">
+      <c r="F47" s="60" t="s">
         <v>320</v>
       </c>
       <c r="G47" t="s">
@@ -14262,7 +14256,7 @@
       <c r="A48" t="s">
         <v>235</v>
       </c>
-      <c r="B48" s="115">
+      <c r="B48" s="61">
         <v>41881</v>
       </c>
       <c r="C48" t="s">
@@ -14274,7 +14268,7 @@
       <c r="E48" t="s">
         <v>238</v>
       </c>
-      <c r="F48" s="114" t="s">
+      <c r="F48" s="60" t="s">
         <v>316</v>
       </c>
       <c r="G48" t="s">
@@ -14309,7 +14303,7 @@
       <c r="A49" t="s">
         <v>239</v>
       </c>
-      <c r="B49" s="115">
+      <c r="B49" s="61">
         <v>41888</v>
       </c>
       <c r="C49" t="s">
@@ -14321,7 +14315,7 @@
       <c r="E49" t="s">
         <v>241</v>
       </c>
-      <c r="F49" s="114" t="s">
+      <c r="F49" s="60" t="s">
         <v>321</v>
       </c>
       <c r="G49" t="s">
@@ -14344,7 +14338,7 @@
       <c r="A50" t="s">
         <v>239</v>
       </c>
-      <c r="B50" s="115">
+      <c r="B50" s="61">
         <v>41888</v>
       </c>
       <c r="C50" t="s">
@@ -14356,7 +14350,7 @@
       <c r="E50" t="s">
         <v>215</v>
       </c>
-      <c r="F50" s="114" t="s">
+      <c r="F50" s="60" t="s">
         <v>322</v>
       </c>
       <c r="G50" t="s">
@@ -14379,7 +14373,7 @@
       <c r="A51" t="s">
         <v>239</v>
       </c>
-      <c r="B51" s="115">
+      <c r="B51" s="61">
         <v>41888</v>
       </c>
       <c r="C51" t="s">
@@ -14391,7 +14385,7 @@
       <c r="E51" t="s">
         <v>242</v>
       </c>
-      <c r="F51" s="114" t="s">
+      <c r="F51" s="60" t="s">
         <v>323</v>
       </c>
       <c r="G51" t="s">
@@ -14426,7 +14420,7 @@
       <c r="A52" t="s">
         <v>243</v>
       </c>
-      <c r="B52" s="115">
+      <c r="B52" s="61">
         <v>41909</v>
       </c>
       <c r="C52" t="s">
@@ -14438,7 +14432,7 @@
       <c r="E52" t="s">
         <v>244</v>
       </c>
-      <c r="F52" s="114" t="s">
+      <c r="F52" s="60" t="s">
         <v>324</v>
       </c>
       <c r="G52" t="s">
@@ -14461,7 +14455,7 @@
       <c r="A53" t="s">
         <v>243</v>
       </c>
-      <c r="B53" s="115">
+      <c r="B53" s="61">
         <v>41909</v>
       </c>
       <c r="C53" t="s">
@@ -14473,7 +14467,7 @@
       <c r="E53" t="s">
         <v>245</v>
       </c>
-      <c r="F53" s="114" t="s">
+      <c r="F53" s="60" t="s">
         <v>325</v>
       </c>
       <c r="G53" t="s">
@@ -14496,7 +14490,7 @@
       <c r="A54" t="s">
         <v>243</v>
       </c>
-      <c r="B54" s="115">
+      <c r="B54" s="61">
         <v>41909</v>
       </c>
       <c r="C54" t="s">
@@ -14508,7 +14502,7 @@
       <c r="E54" t="s">
         <v>246</v>
       </c>
-      <c r="F54" s="114" t="s">
+      <c r="F54" s="60" t="s">
         <v>326</v>
       </c>
       <c r="G54" t="s">
@@ -14543,7 +14537,7 @@
       <c r="A55" t="s">
         <v>247</v>
       </c>
-      <c r="B55" s="115">
+      <c r="B55" s="61">
         <v>41924</v>
       </c>
       <c r="C55" t="s">
@@ -14578,7 +14572,7 @@
       <c r="A56" t="s">
         <v>247</v>
       </c>
-      <c r="B56" s="115">
+      <c r="B56" s="61">
         <v>41924</v>
       </c>
       <c r="C56" t="s">
@@ -14625,7 +14619,7 @@
       <c r="A57" t="s">
         <v>519</v>
       </c>
-      <c r="B57" s="115">
+      <c r="B57" s="61">
         <v>41944</v>
       </c>
       <c r="C57" t="s">
@@ -14637,7 +14631,7 @@
       <c r="E57" t="s">
         <v>252</v>
       </c>
-      <c r="F57" s="114" t="s">
+      <c r="F57" s="60" t="s">
         <v>327</v>
       </c>
       <c r="G57" t="s">
@@ -14673,9 +14667,9 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>520</v>
-      </c>
-      <c r="B58" s="115">
+        <v>519</v>
+      </c>
+      <c r="B58" s="61">
         <v>41944</v>
       </c>
       <c r="C58" t="s">
@@ -14687,7 +14681,7 @@
       <c r="E58" t="s">
         <v>254</v>
       </c>
-      <c r="F58" s="114" t="s">
+      <c r="F58" s="60" t="s">
         <v>328</v>
       </c>
       <c r="G58" t="s">
@@ -14723,9 +14717,9 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>521</v>
-      </c>
-      <c r="B59" s="115">
+        <v>519</v>
+      </c>
+      <c r="B59" s="61">
         <v>41944</v>
       </c>
       <c r="C59" t="s">
@@ -14737,7 +14731,7 @@
       <c r="E59" t="s">
         <v>253</v>
       </c>
-      <c r="F59" s="114" t="s">
+      <c r="F59" s="60" t="s">
         <v>329</v>
       </c>
       <c r="G59" t="s">
@@ -14775,7 +14769,7 @@
       <c r="A60" t="s">
         <v>256</v>
       </c>
-      <c r="B60" s="115">
+      <c r="B60" s="61">
         <v>41946</v>
       </c>
       <c r="C60" t="s">
@@ -14787,7 +14781,7 @@
       <c r="E60" t="s">
         <v>258</v>
       </c>
-      <c r="F60" s="114" t="s">
+      <c r="F60" s="60" t="s">
         <v>330</v>
       </c>
       <c r="G60" t="s">
@@ -14810,7 +14804,7 @@
       <c r="A61" t="s">
         <v>256</v>
       </c>
-      <c r="B61" s="115">
+      <c r="B61" s="61">
         <v>41946</v>
       </c>
       <c r="C61" t="s">
@@ -14822,7 +14816,7 @@
       <c r="E61" t="s">
         <v>192</v>
       </c>
-      <c r="F61" s="114" t="s">
+      <c r="F61" s="60" t="s">
         <v>331</v>
       </c>
       <c r="G61" t="s">
@@ -14845,7 +14839,7 @@
       <c r="A62" t="s">
         <v>256</v>
       </c>
-      <c r="B62" s="115">
+      <c r="B62" s="61">
         <v>41946</v>
       </c>
       <c r="C62" t="s">
@@ -14857,7 +14851,7 @@
       <c r="E62" t="s">
         <v>259</v>
       </c>
-      <c r="F62" s="114" t="s">
+      <c r="F62" s="60" t="s">
         <v>280</v>
       </c>
       <c r="G62" t="s">
@@ -14880,7 +14874,7 @@
       <c r="A63" t="s">
         <v>256</v>
       </c>
-      <c r="B63" s="115">
+      <c r="B63" s="61">
         <v>41946</v>
       </c>
       <c r="C63" t="s">
@@ -14892,7 +14886,7 @@
       <c r="E63" t="s">
         <v>260</v>
       </c>
-      <c r="F63" s="114" t="s">
+      <c r="F63" s="60" t="s">
         <v>332</v>
       </c>
       <c r="G63" t="s">
@@ -14915,7 +14909,7 @@
       <c r="A64" t="s">
         <v>256</v>
       </c>
-      <c r="B64" s="115">
+      <c r="B64" s="61">
         <v>41946</v>
       </c>
       <c r="C64" t="s">
@@ -14927,7 +14921,7 @@
       <c r="E64" t="s">
         <v>152</v>
       </c>
-      <c r="F64" s="114" t="s">
+      <c r="F64" s="60" t="s">
         <v>333</v>
       </c>
       <c r="G64" t="s">
@@ -14950,7 +14944,7 @@
       <c r="A65" t="s">
         <v>261</v>
       </c>
-      <c r="B65" s="115">
+      <c r="B65" s="61">
         <v>41965</v>
       </c>
       <c r="C65" t="s">
@@ -14962,7 +14956,7 @@
       <c r="E65" t="s">
         <v>262</v>
       </c>
-      <c r="F65" s="114" t="s">
+      <c r="F65" s="60" t="s">
         <v>334</v>
       </c>
       <c r="G65" t="s">
@@ -14985,7 +14979,7 @@
       <c r="A66" t="s">
         <v>261</v>
       </c>
-      <c r="B66" s="115">
+      <c r="B66" s="61">
         <v>41965</v>
       </c>
       <c r="C66" t="s">
@@ -14997,7 +14991,7 @@
       <c r="E66" t="s">
         <v>263</v>
       </c>
-      <c r="F66" s="114" t="s">
+      <c r="F66" s="60" t="s">
         <v>335</v>
       </c>
       <c r="G66" t="s">
@@ -15026,7 +15020,7 @@
       <c r="A67" t="s">
         <v>261</v>
       </c>
-      <c r="B67" s="115">
+      <c r="B67" s="61">
         <v>41965</v>
       </c>
       <c r="C67" t="s">
@@ -15038,7 +15032,7 @@
       <c r="E67" t="s">
         <v>339</v>
       </c>
-      <c r="F67" s="114" t="s">
+      <c r="F67" s="60" t="s">
         <v>336</v>
       </c>
       <c r="G67" t="s">
@@ -15073,7 +15067,7 @@
       <c r="A68" t="s">
         <v>264</v>
       </c>
-      <c r="B68" s="115">
+      <c r="B68" s="61">
         <v>42001</v>
       </c>
       <c r="C68" t="s">
@@ -15085,7 +15079,7 @@
       <c r="E68" t="s">
         <v>265</v>
       </c>
-      <c r="F68" s="114" t="s">
+      <c r="F68" s="60" t="s">
         <v>337</v>
       </c>
       <c r="G68" t="s">
@@ -15114,7 +15108,7 @@
       <c r="A69" t="s">
         <v>264</v>
       </c>
-      <c r="B69" s="115">
+      <c r="B69" s="61">
         <v>42001</v>
       </c>
       <c r="C69" t="s">
@@ -15126,7 +15120,7 @@
       <c r="E69" t="s">
         <v>266</v>
       </c>
-      <c r="F69" s="114" t="s">
+      <c r="F69" s="60" t="s">
         <v>338</v>
       </c>
       <c r="G69" t="s">
@@ -15161,7 +15155,7 @@
       <c r="A70" t="s">
         <v>264</v>
       </c>
-      <c r="B70" s="115">
+      <c r="B70" s="61">
         <v>42001</v>
       </c>
       <c r="C70" t="s">
@@ -15173,7 +15167,7 @@
       <c r="E70" t="s">
         <v>219</v>
       </c>
-      <c r="F70" s="114" t="s">
+      <c r="F70" s="60" t="s">
         <v>312</v>
       </c>
       <c r="G70" t="s">
@@ -15295,7 +15289,7 @@
       <c r="A2" t="s">
         <v>340</v>
       </c>
-      <c r="B2" s="115">
+      <c r="B2" s="61">
         <v>42014</v>
       </c>
       <c r="C2" t="s">
@@ -15307,10 +15301,10 @@
       <c r="E2" t="s">
         <v>195</v>
       </c>
-      <c r="F2" s="114" t="s">
+      <c r="F2" s="60" t="s">
         <v>343</v>
       </c>
-      <c r="G2" s="114" t="s">
+      <c r="G2" s="60" t="s">
         <v>149</v>
       </c>
       <c r="H2" t="s">
@@ -15330,7 +15324,7 @@
       <c r="A3" t="s">
         <v>340</v>
       </c>
-      <c r="B3" s="115">
+      <c r="B3" s="61">
         <v>42014</v>
       </c>
       <c r="C3" t="s">
@@ -15342,7 +15336,7 @@
       <c r="E3" t="s">
         <v>341</v>
       </c>
-      <c r="F3" s="114" t="s">
+      <c r="F3" s="60" t="s">
         <v>344</v>
       </c>
       <c r="G3" t="s">
@@ -15365,7 +15359,7 @@
       <c r="A4" t="s">
         <v>340</v>
       </c>
-      <c r="B4" s="115">
+      <c r="B4" s="61">
         <v>42014</v>
       </c>
       <c r="C4" t="s">
@@ -15377,7 +15371,7 @@
       <c r="E4" t="s">
         <v>342</v>
       </c>
-      <c r="F4" s="114" t="s">
+      <c r="F4" s="60" t="s">
         <v>345</v>
       </c>
       <c r="G4" t="s">
@@ -15412,7 +15406,7 @@
       <c r="A5" t="s">
         <v>346</v>
       </c>
-      <c r="B5" s="115">
+      <c r="B5" s="61">
         <v>42043</v>
       </c>
       <c r="C5" t="s">
@@ -15424,7 +15418,7 @@
       <c r="E5" t="s">
         <v>347</v>
       </c>
-      <c r="F5" s="114" t="s">
+      <c r="F5" s="60" t="s">
         <v>349</v>
       </c>
       <c r="G5" t="s">
@@ -15447,7 +15441,7 @@
       <c r="A6" t="s">
         <v>346</v>
       </c>
-      <c r="B6" s="115">
+      <c r="B6" s="61">
         <v>42043</v>
       </c>
       <c r="C6" t="s">
@@ -15459,7 +15453,7 @@
       <c r="E6" t="s">
         <v>205</v>
       </c>
-      <c r="F6" s="114" t="s">
+      <c r="F6" s="60" t="s">
         <v>315</v>
       </c>
       <c r="G6" t="s">
@@ -15482,7 +15476,7 @@
       <c r="A7" t="s">
         <v>346</v>
       </c>
-      <c r="B7" s="115">
+      <c r="B7" s="61">
         <v>42043</v>
       </c>
       <c r="C7" t="s">
@@ -15494,7 +15488,7 @@
       <c r="E7" t="s">
         <v>348</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="60" t="s">
         <v>350</v>
       </c>
       <c r="G7" t="s">
@@ -15529,7 +15523,7 @@
       <c r="A8" t="s">
         <v>352</v>
       </c>
-      <c r="B8" s="115">
+      <c r="B8" s="61">
         <v>42063</v>
       </c>
       <c r="C8" t="s">
@@ -15541,7 +15535,7 @@
       <c r="E8" t="s">
         <v>354</v>
       </c>
-      <c r="F8" s="114" t="s">
+      <c r="F8" s="60" t="s">
         <v>359</v>
       </c>
       <c r="G8" t="s">
@@ -15576,7 +15570,7 @@
       <c r="A9" t="s">
         <v>352</v>
       </c>
-      <c r="B9" s="115">
+      <c r="B9" s="61">
         <v>42063</v>
       </c>
       <c r="C9" t="s">
@@ -15588,7 +15582,7 @@
       <c r="E9" t="s">
         <v>355</v>
       </c>
-      <c r="F9" s="114" t="s">
+      <c r="F9" s="60" t="s">
         <v>360</v>
       </c>
       <c r="G9" t="s">
@@ -15611,7 +15605,7 @@
       <c r="A10" t="s">
         <v>352</v>
       </c>
-      <c r="B10" s="115">
+      <c r="B10" s="61">
         <v>42063</v>
       </c>
       <c r="C10" t="s">
@@ -15623,7 +15617,7 @@
       <c r="E10" t="s">
         <v>356</v>
       </c>
-      <c r="F10" s="114" t="s">
+      <c r="F10" s="60" t="s">
         <v>361</v>
       </c>
       <c r="G10" t="s">
@@ -15646,7 +15640,7 @@
       <c r="A11" t="s">
         <v>352</v>
       </c>
-      <c r="B11" s="115">
+      <c r="B11" s="61">
         <v>42063</v>
       </c>
       <c r="C11" t="s">
@@ -15658,7 +15652,7 @@
       <c r="E11" t="s">
         <v>358</v>
       </c>
-      <c r="F11" s="114" t="s">
+      <c r="F11" s="60" t="s">
         <v>362</v>
       </c>
       <c r="G11" t="s">
@@ -15681,7 +15675,7 @@
       <c r="A12" t="s">
         <v>352</v>
       </c>
-      <c r="B12" s="115">
+      <c r="B12" s="61">
         <v>42063</v>
       </c>
       <c r="C12" t="s">
@@ -15693,7 +15687,7 @@
       <c r="E12" t="s">
         <v>357</v>
       </c>
-      <c r="F12" s="114" t="s">
+      <c r="F12" s="60" t="s">
         <v>363</v>
       </c>
       <c r="G12" t="s">
@@ -15716,7 +15710,7 @@
       <c r="A13" t="s">
         <v>366</v>
       </c>
-      <c r="B13" s="115">
+      <c r="B13" s="61">
         <v>42085</v>
       </c>
       <c r="C13" t="s">
@@ -15728,7 +15722,7 @@
       <c r="E13" t="s">
         <v>367</v>
       </c>
-      <c r="F13" s="114" t="s">
+      <c r="F13" s="60" t="s">
         <v>371</v>
       </c>
       <c r="G13" t="s">
@@ -15751,7 +15745,7 @@
       <c r="A14" t="s">
         <v>366</v>
       </c>
-      <c r="B14" s="115">
+      <c r="B14" s="61">
         <v>42085</v>
       </c>
       <c r="C14" t="s">
@@ -15763,7 +15757,7 @@
       <c r="E14" t="s">
         <v>368</v>
       </c>
-      <c r="F14" s="114" t="s">
+      <c r="F14" s="60" t="s">
         <v>372</v>
       </c>
       <c r="G14" t="s">
@@ -15798,7 +15792,7 @@
       <c r="A15" t="s">
         <v>366</v>
       </c>
-      <c r="B15" s="115">
+      <c r="B15" s="61">
         <v>42085</v>
       </c>
       <c r="C15" t="s">
@@ -15810,7 +15804,7 @@
       <c r="E15" t="s">
         <v>369</v>
       </c>
-      <c r="F15" s="114" t="s">
+      <c r="F15" s="60" t="s">
         <v>373</v>
       </c>
       <c r="G15" t="s">
@@ -15833,7 +15827,7 @@
       <c r="A16" t="s">
         <v>366</v>
       </c>
-      <c r="B16" s="115">
+      <c r="B16" s="61">
         <v>42085</v>
       </c>
       <c r="C16" t="s">
@@ -15845,7 +15839,7 @@
       <c r="E16" t="s">
         <v>370</v>
       </c>
-      <c r="F16" s="114" t="s">
+      <c r="F16" s="60" t="s">
         <v>374</v>
       </c>
       <c r="G16" t="s">
@@ -15880,7 +15874,7 @@
       <c r="A17" t="s">
         <v>375</v>
       </c>
-      <c r="B17" s="115">
+      <c r="B17" s="61">
         <v>42112</v>
       </c>
       <c r="C17" t="s">
@@ -15892,7 +15886,7 @@
       <c r="E17" t="s">
         <v>376</v>
       </c>
-      <c r="F17" s="114" t="s">
+      <c r="F17" s="60" t="s">
         <v>280</v>
       </c>
       <c r="G17" t="s">
@@ -15915,7 +15909,7 @@
       <c r="A18" t="s">
         <v>375</v>
       </c>
-      <c r="B18" s="115">
+      <c r="B18" s="61">
         <v>42112</v>
       </c>
       <c r="C18" t="s">
@@ -15927,7 +15921,7 @@
       <c r="E18" t="s">
         <v>377</v>
       </c>
-      <c r="F18" s="114" t="s">
+      <c r="F18" s="60" t="s">
         <v>379</v>
       </c>
       <c r="G18" t="s">
@@ -15956,7 +15950,7 @@
       <c r="A19" t="s">
         <v>375</v>
       </c>
-      <c r="B19" s="115">
+      <c r="B19" s="61">
         <v>42112</v>
       </c>
       <c r="C19" t="s">
@@ -15968,7 +15962,7 @@
       <c r="E19" t="s">
         <v>378</v>
       </c>
-      <c r="F19" s="114" t="s">
+      <c r="F19" s="60" t="s">
         <v>380</v>
       </c>
       <c r="G19" t="s">
@@ -16003,7 +15997,7 @@
       <c r="A20" t="s">
         <v>375</v>
       </c>
-      <c r="B20" s="115">
+      <c r="B20" s="61">
         <v>42112</v>
       </c>
       <c r="C20" t="s">
@@ -16015,7 +16009,7 @@
       <c r="E20" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="114" t="s">
+      <c r="F20" s="60" t="s">
         <v>381</v>
       </c>
       <c r="G20" t="s">
@@ -16038,7 +16032,7 @@
       <c r="A21" t="s">
         <v>382</v>
       </c>
-      <c r="B21" s="115">
+      <c r="B21" s="61">
         <v>42147</v>
       </c>
       <c r="C21" t="s">
@@ -16050,7 +16044,7 @@
       <c r="E21" t="s">
         <v>383</v>
       </c>
-      <c r="F21" s="114" t="s">
+      <c r="F21" s="60" t="s">
         <v>388</v>
       </c>
       <c r="G21" t="s">
@@ -16073,7 +16067,7 @@
       <c r="A22" t="s">
         <v>382</v>
       </c>
-      <c r="B22" s="115">
+      <c r="B22" s="61">
         <v>42147</v>
       </c>
       <c r="C22" t="s">
@@ -16085,7 +16079,7 @@
       <c r="E22" t="s">
         <v>384</v>
       </c>
-      <c r="F22" s="114" t="s">
+      <c r="F22" s="60" t="s">
         <v>389</v>
       </c>
       <c r="G22" t="s">
@@ -16120,7 +16114,7 @@
       <c r="A23" t="s">
         <v>382</v>
       </c>
-      <c r="B23" s="115">
+      <c r="B23" s="61">
         <v>42147</v>
       </c>
       <c r="C23" t="s">
@@ -16132,7 +16126,7 @@
       <c r="E23" t="s">
         <v>385</v>
       </c>
-      <c r="F23" s="114" t="s">
+      <c r="F23" s="60" t="s">
         <v>390</v>
       </c>
       <c r="G23" t="s">
@@ -16155,7 +16149,7 @@
       <c r="A24" t="s">
         <v>382</v>
       </c>
-      <c r="B24" s="115">
+      <c r="B24" s="61">
         <v>42147</v>
       </c>
       <c r="C24" t="s">
@@ -16167,7 +16161,7 @@
       <c r="E24" t="s">
         <v>386</v>
       </c>
-      <c r="F24" s="114" t="s">
+      <c r="F24" s="60" t="s">
         <v>319</v>
       </c>
       <c r="G24" t="s">
@@ -16190,7 +16184,7 @@
       <c r="A25" t="s">
         <v>382</v>
       </c>
-      <c r="B25" s="115">
+      <c r="B25" s="61">
         <v>42147</v>
       </c>
       <c r="C25" t="s">
@@ -16202,7 +16196,7 @@
       <c r="E25" t="s">
         <v>387</v>
       </c>
-      <c r="F25" s="114" t="s">
+      <c r="F25" s="60" t="s">
         <v>391</v>
       </c>
       <c r="G25" t="s">
@@ -16225,7 +16219,7 @@
       <c r="A26" t="s">
         <v>392</v>
       </c>
-      <c r="B26" s="115">
+      <c r="B26" s="61">
         <v>42162</v>
       </c>
       <c r="C26" t="s">
@@ -16237,7 +16231,7 @@
       <c r="E26" t="s">
         <v>393</v>
       </c>
-      <c r="F26" s="114" t="s">
+      <c r="F26" s="60" t="s">
         <v>396</v>
       </c>
       <c r="G26" t="s">
@@ -16260,7 +16254,7 @@
       <c r="A27" t="s">
         <v>392</v>
       </c>
-      <c r="B27" s="115">
+      <c r="B27" s="61">
         <v>42162</v>
       </c>
       <c r="C27" t="s">
@@ -16272,7 +16266,7 @@
       <c r="E27" t="s">
         <v>178</v>
       </c>
-      <c r="F27" s="114" t="s">
+      <c r="F27" s="60" t="s">
         <v>397</v>
       </c>
       <c r="G27" t="s">
@@ -16295,7 +16289,7 @@
       <c r="A28" t="s">
         <v>392</v>
       </c>
-      <c r="B28" s="115">
+      <c r="B28" s="61">
         <v>42162</v>
       </c>
       <c r="C28" t="s">
@@ -16307,7 +16301,7 @@
       <c r="E28" t="s">
         <v>394</v>
       </c>
-      <c r="F28" s="114" t="s">
+      <c r="F28" s="60" t="s">
         <v>398</v>
       </c>
       <c r="G28" t="s">
@@ -16330,7 +16324,7 @@
       <c r="A29" t="s">
         <v>392</v>
       </c>
-      <c r="B29" s="115">
+      <c r="B29" s="61">
         <v>42162</v>
       </c>
       <c r="C29" t="s">
@@ -16342,7 +16336,7 @@
       <c r="E29" t="s">
         <v>395</v>
       </c>
-      <c r="F29" s="114" t="s">
+      <c r="F29" s="60" t="s">
         <v>399</v>
       </c>
       <c r="G29" t="s">
@@ -16377,7 +16371,7 @@
       <c r="A30" t="s">
         <v>400</v>
       </c>
-      <c r="B30" s="115">
+      <c r="B30" s="61">
         <v>42175</v>
       </c>
       <c r="C30" t="s">
@@ -16389,7 +16383,7 @@
       <c r="E30" t="s">
         <v>401</v>
       </c>
-      <c r="F30" s="114" t="s">
+      <c r="F30" s="60" t="s">
         <v>404</v>
       </c>
       <c r="G30" t="s">
@@ -16418,7 +16412,7 @@
       <c r="A31" t="s">
         <v>400</v>
       </c>
-      <c r="B31" s="115">
+      <c r="B31" s="61">
         <v>42175</v>
       </c>
       <c r="C31" t="s">
@@ -16430,7 +16424,7 @@
       <c r="E31" t="s">
         <v>402</v>
       </c>
-      <c r="F31" s="114" t="s">
+      <c r="F31" s="60" t="s">
         <v>288</v>
       </c>
       <c r="G31" t="s">
@@ -16453,7 +16447,7 @@
       <c r="A32" t="s">
         <v>400</v>
       </c>
-      <c r="B32" s="115">
+      <c r="B32" s="61">
         <v>42175</v>
       </c>
       <c r="C32" t="s">
@@ -16465,7 +16459,7 @@
       <c r="E32" t="s">
         <v>184</v>
       </c>
-      <c r="F32" s="114" t="s">
+      <c r="F32" s="60" t="s">
         <v>405</v>
       </c>
       <c r="G32" t="s">
@@ -16488,7 +16482,7 @@
       <c r="A33" t="s">
         <v>400</v>
       </c>
-      <c r="B33" s="115">
+      <c r="B33" s="61">
         <v>42175</v>
       </c>
       <c r="C33" t="s">
@@ -16500,7 +16494,7 @@
       <c r="E33" t="s">
         <v>403</v>
       </c>
-      <c r="F33" s="114" t="s">
+      <c r="F33" s="60" t="s">
         <v>406</v>
       </c>
       <c r="G33" t="s">
@@ -16535,7 +16529,7 @@
       <c r="A34" t="s">
         <v>407</v>
       </c>
-      <c r="B34" s="115">
+      <c r="B34" s="61">
         <v>42189</v>
       </c>
       <c r="C34" t="s">
@@ -16547,7 +16541,7 @@
       <c r="E34" t="s">
         <v>408</v>
       </c>
-      <c r="F34" s="114" t="s">
+      <c r="F34" s="60" t="s">
         <v>410</v>
       </c>
       <c r="G34" t="s">
@@ -16570,7 +16564,7 @@
       <c r="A35" t="s">
         <v>407</v>
       </c>
-      <c r="B35" s="115">
+      <c r="B35" s="61">
         <v>42189</v>
       </c>
       <c r="C35" t="s">
@@ -16582,7 +16576,7 @@
       <c r="E35" t="s">
         <v>402</v>
       </c>
-      <c r="F35" s="114" t="s">
+      <c r="F35" s="60" t="s">
         <v>388</v>
       </c>
       <c r="G35" t="s">
@@ -16608,7 +16602,7 @@
       <c r="A36" t="s">
         <v>407</v>
       </c>
-      <c r="B36" s="115">
+      <c r="B36" s="61">
         <v>42189</v>
       </c>
       <c r="C36" t="s">
@@ -16620,7 +16614,7 @@
       <c r="E36" t="s">
         <v>184</v>
       </c>
-      <c r="F36" s="114" t="s">
+      <c r="F36" s="60" t="s">
         <v>411</v>
       </c>
       <c r="G36" t="s">
@@ -16646,7 +16640,7 @@
       <c r="A37" t="s">
         <v>407</v>
       </c>
-      <c r="B37" s="115">
+      <c r="B37" s="61">
         <v>42189</v>
       </c>
       <c r="C37" t="s">
@@ -16658,7 +16652,7 @@
       <c r="E37" t="s">
         <v>409</v>
       </c>
-      <c r="F37" s="114" t="s">
+      <c r="F37" s="60" t="s">
         <v>412</v>
       </c>
       <c r="G37" t="s">
@@ -16693,7 +16687,7 @@
       <c r="A38" t="s">
         <v>414</v>
       </c>
-      <c r="B38" s="115">
+      <c r="B38" s="61">
         <v>42203</v>
       </c>
       <c r="C38" t="s">
@@ -16705,7 +16699,7 @@
       <c r="E38" t="s">
         <v>416</v>
       </c>
-      <c r="F38" s="114" t="s">
+      <c r="F38" s="60" t="s">
         <v>420</v>
       </c>
       <c r="G38" t="s">
@@ -16734,7 +16728,7 @@
       <c r="A39" t="s">
         <v>414</v>
       </c>
-      <c r="B39" s="115">
+      <c r="B39" s="61">
         <v>42203</v>
       </c>
       <c r="C39" t="s">
@@ -16746,7 +16740,7 @@
       <c r="E39" t="s">
         <v>417</v>
       </c>
-      <c r="F39" s="114" t="s">
+      <c r="F39" s="60" t="s">
         <v>372</v>
       </c>
       <c r="G39" t="s">
@@ -16781,7 +16775,7 @@
       <c r="A40" t="s">
         <v>414</v>
       </c>
-      <c r="B40" s="115">
+      <c r="B40" s="61">
         <v>42203</v>
       </c>
       <c r="C40" t="s">
@@ -16793,7 +16787,7 @@
       <c r="E40" t="s">
         <v>418</v>
       </c>
-      <c r="F40" s="114" t="s">
+      <c r="F40" s="60" t="s">
         <v>421</v>
       </c>
       <c r="G40" t="s">
@@ -16819,7 +16813,7 @@
       <c r="A41" t="s">
         <v>414</v>
       </c>
-      <c r="B41" s="115">
+      <c r="B41" s="61">
         <v>42203</v>
       </c>
       <c r="C41" t="s">
@@ -16831,7 +16825,7 @@
       <c r="E41" t="s">
         <v>419</v>
       </c>
-      <c r="F41" s="114" t="s">
+      <c r="F41" s="60" t="s">
         <v>422</v>
       </c>
       <c r="G41" t="s">
@@ -16857,7 +16851,7 @@
       <c r="A42" t="s">
         <v>424</v>
       </c>
-      <c r="B42" s="115">
+      <c r="B42" s="61">
         <v>42208</v>
       </c>
       <c r="C42" t="s">
@@ -16869,7 +16863,7 @@
       <c r="E42" t="s">
         <v>427</v>
       </c>
-      <c r="F42" s="114" t="s">
+      <c r="F42" s="60" t="s">
         <v>398</v>
       </c>
       <c r="G42" t="s">
@@ -16892,7 +16886,7 @@
       <c r="A43" t="s">
         <v>424</v>
       </c>
-      <c r="B43" s="115">
+      <c r="B43" s="61">
         <v>42208</v>
       </c>
       <c r="C43" t="s">
@@ -16904,7 +16898,7 @@
       <c r="E43" t="s">
         <v>428</v>
       </c>
-      <c r="F43" s="114" t="s">
+      <c r="F43" s="60" t="s">
         <v>430</v>
       </c>
       <c r="G43" t="s">
@@ -16927,7 +16921,7 @@
       <c r="A44" t="s">
         <v>424</v>
       </c>
-      <c r="B44" s="115">
+      <c r="B44" s="61">
         <v>42208</v>
       </c>
       <c r="C44" t="s">
@@ -16939,7 +16933,7 @@
       <c r="E44" t="s">
         <v>429</v>
       </c>
-      <c r="F44" s="114" t="s">
+      <c r="F44" s="60" t="s">
         <v>431</v>
       </c>
       <c r="G44" t="s">
@@ -16986,7 +16980,7 @@
       <c r="A45" t="s">
         <v>436</v>
       </c>
-      <c r="B45" s="115">
+      <c r="B45" s="61">
         <v>42224</v>
       </c>
       <c r="C45" t="s">
@@ -16998,7 +16992,7 @@
       <c r="E45" t="s">
         <v>262</v>
       </c>
-      <c r="F45" s="114" t="s">
+      <c r="F45" s="60" t="s">
         <v>439</v>
       </c>
       <c r="G45" t="s">
@@ -17024,7 +17018,7 @@
       <c r="A46" t="s">
         <v>436</v>
       </c>
-      <c r="B46" s="115">
+      <c r="B46" s="61">
         <v>42224</v>
       </c>
       <c r="C46" t="s">
@@ -17036,7 +17030,7 @@
       <c r="E46" t="s">
         <v>394</v>
       </c>
-      <c r="F46" s="114" t="s">
+      <c r="F46" s="60" t="s">
         <v>440</v>
       </c>
       <c r="G46" t="s">
@@ -17062,7 +17056,7 @@
       <c r="A47" t="s">
         <v>436</v>
       </c>
-      <c r="B47" s="115">
+      <c r="B47" s="61">
         <v>42224</v>
       </c>
       <c r="C47" t="s">
@@ -17074,7 +17068,7 @@
       <c r="E47" t="s">
         <v>437</v>
       </c>
-      <c r="F47" s="114" t="s">
+      <c r="F47" s="60" t="s">
         <v>441</v>
       </c>
       <c r="G47" t="s">
@@ -17103,7 +17097,7 @@
       <c r="A48" t="s">
         <v>436</v>
       </c>
-      <c r="B48" s="115">
+      <c r="B48" s="61">
         <v>42224</v>
       </c>
       <c r="C48" t="s">
@@ -17115,7 +17109,7 @@
       <c r="E48" t="s">
         <v>438</v>
       </c>
-      <c r="F48" s="114" t="s">
+      <c r="F48" s="60" t="s">
         <v>442</v>
       </c>
       <c r="G48" t="s">
@@ -17153,7 +17147,7 @@
       <c r="A49" t="s">
         <v>436</v>
       </c>
-      <c r="B49" s="115">
+      <c r="B49" s="61">
         <v>42224</v>
       </c>
       <c r="C49" t="s">
@@ -17165,7 +17159,7 @@
       <c r="E49" t="s">
         <v>214</v>
       </c>
-      <c r="F49" s="114" t="s">
+      <c r="F49" s="60" t="s">
         <v>443</v>
       </c>
       <c r="G49" t="s">
@@ -17191,7 +17185,7 @@
       <c r="A50" t="s">
         <v>447</v>
       </c>
-      <c r="B50" s="115">
+      <c r="B50" s="61">
         <v>42245</v>
       </c>
       <c r="C50" t="s">
@@ -17203,7 +17197,7 @@
       <c r="E50" t="s">
         <v>448</v>
       </c>
-      <c r="F50" s="114" t="s">
+      <c r="F50" s="60" t="s">
         <v>452</v>
       </c>
       <c r="G50" t="s">
@@ -17226,7 +17220,7 @@
       <c r="A51" t="s">
         <v>447</v>
       </c>
-      <c r="B51" s="115">
+      <c r="B51" s="61">
         <v>42245</v>
       </c>
       <c r="C51" t="s">
@@ -17238,7 +17232,7 @@
       <c r="E51" t="s">
         <v>449</v>
       </c>
-      <c r="F51" s="114" t="s">
+      <c r="F51" s="60" t="s">
         <v>453</v>
       </c>
       <c r="G51" t="s">
@@ -17261,7 +17255,7 @@
       <c r="A52" t="s">
         <v>447</v>
       </c>
-      <c r="B52" s="115">
+      <c r="B52" s="61">
         <v>42245</v>
       </c>
       <c r="C52" t="s">
@@ -17273,7 +17267,7 @@
       <c r="E52" t="s">
         <v>450</v>
       </c>
-      <c r="F52" s="114" t="s">
+      <c r="F52" s="60" t="s">
         <v>299</v>
       </c>
       <c r="G52" t="s">
@@ -17296,7 +17290,7 @@
       <c r="A53" t="s">
         <v>447</v>
       </c>
-      <c r="B53" s="115">
+      <c r="B53" s="61">
         <v>42245</v>
       </c>
       <c r="C53" t="s">
@@ -17308,7 +17302,7 @@
       <c r="E53" t="s">
         <v>451</v>
       </c>
-      <c r="F53" s="114" t="s">
+      <c r="F53" s="60" t="s">
         <v>431</v>
       </c>
       <c r="G53" t="s">
@@ -17343,7 +17337,7 @@
       <c r="A54" t="s">
         <v>455</v>
       </c>
-      <c r="B54" s="115">
+      <c r="B54" s="61">
         <v>42269</v>
       </c>
       <c r="C54" t="s">
@@ -17355,7 +17349,7 @@
       <c r="E54" t="s">
         <v>456</v>
       </c>
-      <c r="F54" s="114" t="s">
+      <c r="F54" s="60" t="s">
         <v>282</v>
       </c>
       <c r="G54" t="s">
@@ -17378,7 +17372,7 @@
       <c r="A55" t="s">
         <v>455</v>
       </c>
-      <c r="B55" s="115">
+      <c r="B55" s="61">
         <v>42269</v>
       </c>
       <c r="C55" t="s">
@@ -17390,7 +17384,7 @@
       <c r="E55" t="s">
         <v>457</v>
       </c>
-      <c r="F55" s="114" t="s">
+      <c r="F55" s="60" t="s">
         <v>331</v>
       </c>
       <c r="G55" t="s">
@@ -17413,7 +17407,7 @@
       <c r="A56" t="s">
         <v>455</v>
       </c>
-      <c r="B56" s="115">
+      <c r="B56" s="61">
         <v>42269</v>
       </c>
       <c r="C56" t="s">
@@ -17425,7 +17419,7 @@
       <c r="E56" t="s">
         <v>458</v>
       </c>
-      <c r="F56" s="114" t="s">
+      <c r="F56" s="60" t="s">
         <v>295</v>
       </c>
       <c r="G56" t="s">
@@ -17448,7 +17442,7 @@
       <c r="A57" t="s">
         <v>455</v>
       </c>
-      <c r="B57" s="115">
+      <c r="B57" s="61">
         <v>42269</v>
       </c>
       <c r="C57" t="s">
@@ -17460,7 +17454,7 @@
       <c r="E57" t="s">
         <v>459</v>
       </c>
-      <c r="F57" s="114" t="s">
+      <c r="F57" s="60" t="s">
         <v>461</v>
       </c>
       <c r="G57" t="s">
@@ -17495,7 +17489,7 @@
       <c r="A58" t="s">
         <v>455</v>
       </c>
-      <c r="B58" s="115">
+      <c r="B58" s="61">
         <v>42269</v>
       </c>
       <c r="C58" t="s">
@@ -17507,7 +17501,7 @@
       <c r="E58" t="s">
         <v>460</v>
       </c>
-      <c r="F58" s="114" t="s">
+      <c r="F58" s="60" t="s">
         <v>462</v>
       </c>
       <c r="G58" t="s">
@@ -17530,7 +17524,7 @@
       <c r="A59" t="s">
         <v>464</v>
       </c>
-      <c r="B59" s="115">
+      <c r="B59" s="61">
         <v>42289</v>
       </c>
       <c r="C59" t="s">
@@ -17542,7 +17536,7 @@
       <c r="E59" t="s">
         <v>367</v>
       </c>
-      <c r="F59" s="114" t="s">
+      <c r="F59" s="60" t="s">
         <v>391</v>
       </c>
       <c r="G59" t="s">
@@ -17565,7 +17559,7 @@
       <c r="A60" t="s">
         <v>464</v>
       </c>
-      <c r="B60" s="115">
+      <c r="B60" s="61">
         <v>42289</v>
       </c>
       <c r="C60" t="s">
@@ -17577,7 +17571,7 @@
       <c r="E60" t="s">
         <v>465</v>
       </c>
-      <c r="F60" s="114" t="s">
+      <c r="F60" s="60" t="s">
         <v>311</v>
       </c>
       <c r="G60" t="s">
@@ -17600,7 +17594,7 @@
       <c r="A61" t="s">
         <v>464</v>
       </c>
-      <c r="B61" s="115">
+      <c r="B61" s="61">
         <v>42289</v>
       </c>
       <c r="C61" t="s">
@@ -17612,7 +17606,7 @@
       <c r="E61" t="s">
         <v>466</v>
       </c>
-      <c r="F61" s="114" t="s">
+      <c r="F61" s="60" t="s">
         <v>468</v>
       </c>
       <c r="G61" t="s">
@@ -17641,7 +17635,7 @@
       <c r="A62" t="s">
         <v>464</v>
       </c>
-      <c r="B62" s="115">
+      <c r="B62" s="61">
         <v>42289</v>
       </c>
       <c r="C62" t="s">
@@ -17653,7 +17647,7 @@
       <c r="E62" t="s">
         <v>467</v>
       </c>
-      <c r="F62" s="114" t="s">
+      <c r="F62" s="60" t="s">
         <v>469</v>
       </c>
       <c r="G62" t="s">
@@ -17700,7 +17694,7 @@
       <c r="A63" t="s">
         <v>470</v>
       </c>
-      <c r="B63" s="115">
+      <c r="B63" s="61">
         <v>42295</v>
       </c>
       <c r="C63" t="s">
@@ -17712,7 +17706,7 @@
       <c r="E63" t="s">
         <v>472</v>
       </c>
-      <c r="F63" s="114" t="s">
+      <c r="F63" s="60" t="s">
         <v>473</v>
       </c>
       <c r="G63" t="s">
@@ -17750,7 +17744,7 @@
       <c r="A64" t="s">
         <v>475</v>
       </c>
-      <c r="B64" s="115">
+      <c r="B64" s="61">
         <v>42301</v>
       </c>
       <c r="C64" t="s">
@@ -17762,7 +17756,7 @@
       <c r="E64" t="s">
         <v>476</v>
       </c>
-      <c r="F64" s="114" t="s">
+      <c r="F64" s="60" t="s">
         <v>479</v>
       </c>
       <c r="G64" t="s">
@@ -17791,7 +17785,7 @@
       <c r="A65" t="s">
         <v>475</v>
       </c>
-      <c r="B65" s="115">
+      <c r="B65" s="61">
         <v>42301</v>
       </c>
       <c r="C65" t="s">
@@ -17803,7 +17797,7 @@
       <c r="E65" t="s">
         <v>477</v>
       </c>
-      <c r="F65" s="114" t="s">
+      <c r="F65" s="60" t="s">
         <v>480</v>
       </c>
       <c r="G65" t="s">
@@ -17850,7 +17844,7 @@
       <c r="A66" t="s">
         <v>475</v>
       </c>
-      <c r="B66" s="115">
+      <c r="B66" s="61">
         <v>42301</v>
       </c>
       <c r="C66" t="s">
@@ -17862,7 +17856,7 @@
       <c r="E66" t="s">
         <v>478</v>
       </c>
-      <c r="F66" s="114" t="s">
+      <c r="F66" s="60" t="s">
         <v>481</v>
       </c>
       <c r="G66" t="s">
@@ -17885,7 +17879,7 @@
       <c r="A67" t="s">
         <v>475</v>
       </c>
-      <c r="B67" s="115">
+      <c r="B67" s="61">
         <v>42301</v>
       </c>
       <c r="C67" t="s">
@@ -17897,7 +17891,7 @@
       <c r="E67" t="s">
         <v>478</v>
       </c>
-      <c r="F67" s="114" t="s">
+      <c r="F67" s="60" t="s">
         <v>482</v>
       </c>
       <c r="G67" t="s">
@@ -17923,7 +17917,7 @@
       <c r="A68" t="s">
         <v>475</v>
       </c>
-      <c r="B68" s="115">
+      <c r="B68" s="61">
         <v>42301</v>
       </c>
       <c r="C68" t="s">
@@ -17935,7 +17929,7 @@
       <c r="E68" t="s">
         <v>219</v>
       </c>
-      <c r="F68" s="114" t="s">
+      <c r="F68" s="60" t="s">
         <v>280</v>
       </c>
       <c r="G68" t="s">
@@ -17961,7 +17955,7 @@
       <c r="A69" t="s">
         <v>486</v>
       </c>
-      <c r="B69" s="115">
+      <c r="B69" s="61">
         <v>42315</v>
       </c>
       <c r="C69" t="s">
@@ -17973,7 +17967,7 @@
       <c r="E69" t="s">
         <v>488</v>
       </c>
-      <c r="F69" s="114" t="s">
+      <c r="F69" s="60" t="s">
         <v>492</v>
       </c>
       <c r="G69" t="s">
@@ -18002,7 +17996,7 @@
       <c r="A70" t="s">
         <v>486</v>
       </c>
-      <c r="B70" s="115">
+      <c r="B70" s="61">
         <v>42315</v>
       </c>
       <c r="C70" t="s">
@@ -18014,7 +18008,7 @@
       <c r="E70" t="s">
         <v>489</v>
       </c>
-      <c r="F70" s="114" t="s">
+      <c r="F70" s="60" t="s">
         <v>493</v>
       </c>
       <c r="G70" t="s">
@@ -18061,7 +18055,7 @@
       <c r="A71" t="s">
         <v>486</v>
       </c>
-      <c r="B71" s="115">
+      <c r="B71" s="61">
         <v>42315</v>
       </c>
       <c r="C71" t="s">
@@ -18073,7 +18067,7 @@
       <c r="E71" t="s">
         <v>490</v>
       </c>
-      <c r="F71" s="114" t="s">
+      <c r="F71" s="60" t="s">
         <v>494</v>
       </c>
       <c r="G71" t="s">
@@ -18108,7 +18102,7 @@
       <c r="A72" t="s">
         <v>486</v>
       </c>
-      <c r="B72" s="115">
+      <c r="B72" s="61">
         <v>42315</v>
       </c>
       <c r="C72" t="s">
@@ -18120,7 +18114,7 @@
       <c r="E72" t="s">
         <v>491</v>
       </c>
-      <c r="F72" s="114" t="s">
+      <c r="F72" s="60" t="s">
         <v>495</v>
       </c>
       <c r="G72" t="s">
@@ -18146,7 +18140,7 @@
       <c r="A73" t="s">
         <v>498</v>
       </c>
-      <c r="B73" s="115">
+      <c r="B73" s="61">
         <v>42360</v>
       </c>
       <c r="C73" t="s">
@@ -18158,7 +18152,7 @@
       <c r="E73" t="s">
         <v>500</v>
       </c>
-      <c r="F73" s="114" t="s">
+      <c r="F73" s="60" t="s">
         <v>505</v>
       </c>
       <c r="G73" t="s">
@@ -18184,7 +18178,7 @@
       <c r="A74" t="s">
         <v>498</v>
       </c>
-      <c r="B74" s="115">
+      <c r="B74" s="61">
         <v>42360</v>
       </c>
       <c r="C74" t="s">
@@ -18196,7 +18190,7 @@
       <c r="E74" t="s">
         <v>501</v>
       </c>
-      <c r="F74" s="114" t="s">
+      <c r="F74" s="60" t="s">
         <v>506</v>
       </c>
       <c r="G74" t="s">
@@ -18219,7 +18213,7 @@
       <c r="A75" t="s">
         <v>498</v>
       </c>
-      <c r="B75" s="115">
+      <c r="B75" s="61">
         <v>42360</v>
       </c>
       <c r="C75" t="s">
@@ -18231,7 +18225,7 @@
       <c r="E75" t="s">
         <v>502</v>
       </c>
-      <c r="F75" s="114" t="s">
+      <c r="F75" s="60" t="s">
         <v>507</v>
       </c>
       <c r="G75" t="s">
@@ -18260,7 +18254,7 @@
       <c r="A76" t="s">
         <v>498</v>
       </c>
-      <c r="B76" s="115">
+      <c r="B76" s="61">
         <v>42360</v>
       </c>
       <c r="C76" t="s">
@@ -18272,7 +18266,7 @@
       <c r="E76" t="s">
         <v>503</v>
       </c>
-      <c r="F76" s="114" t="s">
+      <c r="F76" s="60" t="s">
         <v>508</v>
       </c>
       <c r="G76" t="s">
@@ -18307,7 +18301,7 @@
       <c r="A77" t="s">
         <v>498</v>
       </c>
-      <c r="B77" s="115">
+      <c r="B77" s="61">
         <v>42360</v>
       </c>
       <c r="C77" t="s">
@@ -18319,7 +18313,7 @@
       <c r="E77" t="s">
         <v>504</v>
       </c>
-      <c r="F77" s="114" t="s">
+      <c r="F77" s="60" t="s">
         <v>508</v>
       </c>
       <c r="G77" t="s">
@@ -18342,7 +18336,7 @@
       <c r="A78" t="s">
         <v>498</v>
       </c>
-      <c r="B78" s="115">
+      <c r="B78" s="61">
         <v>42360</v>
       </c>
       <c r="C78" t="s">
@@ -18354,7 +18348,7 @@
       <c r="E78" t="s">
         <v>152</v>
       </c>
-      <c r="F78" s="114" t="s">
+      <c r="F78" s="60" t="s">
         <v>509</v>
       </c>
       <c r="G78" t="s">

</xml_diff>

<commit_message>
Not sure if any changes or not to spreadsheet
</commit_message>
<xml_diff>
--- a/TJPW Metrics.xlsx
+++ b/TJPW Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2134,108 +2134,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2295,6 +2193,108 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2689,52 +2689,52 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="100" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="101"/>
-      <c r="I2" s="102" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="104"/>
-      <c r="M2" s="105" t="s">
+      <c r="G2" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
-      <c r="P2" s="106"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="108" t="s">
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="109"/>
-      <c r="T2" s="109"/>
-      <c r="U2" s="109"/>
-      <c r="V2" s="110"/>
-      <c r="W2" s="111" t="s">
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="112"/>
-      <c r="Y2" s="112"/>
-      <c r="Z2" s="112"/>
-      <c r="AA2" s="112"/>
-      <c r="AB2" s="112"/>
-      <c r="AC2" s="112"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="112"/>
-      <c r="AF2" s="113"/>
-      <c r="AG2" s="114" t="s">
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="78"/>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+      <c r="AE2" s="78"/>
+      <c r="AF2" s="79"/>
+      <c r="AG2" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="AH2" s="115"/>
-      <c r="AI2" s="115"/>
-      <c r="AJ2" s="115"/>
-      <c r="AK2" s="115"/>
-      <c r="AL2" s="115"/>
-      <c r="AM2" s="115"/>
-      <c r="AN2" s="116"/>
+      <c r="AH2" s="81"/>
+      <c r="AI2" s="81"/>
+      <c r="AJ2" s="81"/>
+      <c r="AK2" s="81"/>
+      <c r="AL2" s="81"/>
+      <c r="AM2" s="81"/>
+      <c r="AN2" s="82"/>
       <c r="AO2" s="83" t="s">
         <v>7</v>
       </c>
@@ -2771,15 +2771,15 @@
       </c>
       <c r="BK2" s="95"/>
       <c r="BL2" s="96"/>
-      <c r="BM2" s="97" t="s">
+      <c r="BM2" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="BN2" s="98"/>
-      <c r="BO2" s="98"/>
-      <c r="BP2" s="98"/>
-      <c r="BQ2" s="98"/>
-      <c r="BR2" s="98"/>
-      <c r="BS2" s="99"/>
+      <c r="BN2" s="64"/>
+      <c r="BO2" s="64"/>
+      <c r="BP2" s="64"/>
+      <c r="BQ2" s="64"/>
+      <c r="BR2" s="64"/>
+      <c r="BS2" s="65"/>
     </row>
     <row r="3" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
@@ -2800,18 +2800,18 @@
       <c r="F3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="76">
+      <c r="G3" s="99">
         <v>2020</v>
       </c>
-      <c r="H3" s="77"/>
-      <c r="I3" s="78" t="s">
+      <c r="H3" s="100"/>
+      <c r="I3" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="79"/>
-      <c r="K3" s="80" t="s">
+      <c r="J3" s="102"/>
+      <c r="K3" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="78"/>
+      <c r="L3" s="101"/>
       <c r="M3" s="14" t="s">
         <v>21</v>
       </c>
@@ -2842,74 +2842,74 @@
       <c r="V3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="81" t="s">
+      <c r="W3" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="82"/>
-      <c r="Y3" s="81" t="s">
+      <c r="X3" s="105"/>
+      <c r="Y3" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="Z3" s="72"/>
-      <c r="AA3" s="72" t="s">
+      <c r="Z3" s="106"/>
+      <c r="AA3" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="72"/>
-      <c r="AC3" s="72" t="s">
+      <c r="AB3" s="106"/>
+      <c r="AC3" s="106" t="s">
         <v>29</v>
       </c>
-      <c r="AD3" s="72"/>
-      <c r="AE3" s="72" t="s">
+      <c r="AD3" s="106"/>
+      <c r="AE3" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="AF3" s="72"/>
-      <c r="AG3" s="73" t="s">
+      <c r="AF3" s="106"/>
+      <c r="AG3" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="74"/>
-      <c r="AI3" s="75" t="s">
+      <c r="AH3" s="98"/>
+      <c r="AI3" s="107" t="s">
         <v>32</v>
       </c>
-      <c r="AJ3" s="73"/>
-      <c r="AK3" s="73" t="s">
+      <c r="AJ3" s="97"/>
+      <c r="AK3" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="AL3" s="73"/>
-      <c r="AM3" s="73" t="s">
+      <c r="AL3" s="97"/>
+      <c r="AM3" s="97" t="s">
         <v>34</v>
       </c>
-      <c r="AN3" s="74"/>
-      <c r="AO3" s="66" t="s">
+      <c r="AN3" s="98"/>
+      <c r="AO3" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="AP3" s="67"/>
-      <c r="AQ3" s="66" t="s">
+      <c r="AP3" s="112"/>
+      <c r="AQ3" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="AR3" s="68"/>
-      <c r="AS3" s="68" t="s">
+      <c r="AR3" s="113"/>
+      <c r="AS3" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="AT3" s="67"/>
-      <c r="AU3" s="69" t="s">
+      <c r="AT3" s="112"/>
+      <c r="AU3" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="AV3" s="70"/>
-      <c r="AW3" s="71" t="s">
+      <c r="AV3" s="115"/>
+      <c r="AW3" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="AX3" s="63"/>
-      <c r="AY3" s="63" t="s">
+      <c r="AX3" s="108"/>
+      <c r="AY3" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="AZ3" s="63"/>
-      <c r="BA3" s="63" t="s">
+      <c r="AZ3" s="108"/>
+      <c r="BA3" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="BB3" s="63"/>
-      <c r="BC3" s="64" t="s">
+      <c r="BB3" s="108"/>
+      <c r="BC3" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="BD3" s="65"/>
+      <c r="BD3" s="110"/>
       <c r="BE3" s="22" t="s">
         <v>19</v>
       </c>
@@ -11800,6 +11800,26 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="AO3:AP3"/>
+    <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AY3:AZ3"/>
+    <mergeCell ref="AM3:AN3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AG3:AH3"/>
+    <mergeCell ref="AI3:AJ3"/>
+    <mergeCell ref="AK3:AL3"/>
     <mergeCell ref="BM2:BS2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:L2"/>
@@ -11812,26 +11832,6 @@
     <mergeCell ref="AW2:BD2"/>
     <mergeCell ref="BE2:BH2"/>
     <mergeCell ref="BJ2:BL2"/>
-    <mergeCell ref="AM3:AN3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AG3:AH3"/>
-    <mergeCell ref="AI3:AJ3"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="BA3:BB3"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="AO3:AP3"/>
-    <mergeCell ref="AQ3:AR3"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AW3:AX3"/>
-    <mergeCell ref="AY3:AZ3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12411,7 +12411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="H40" workbookViewId="0">
       <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
@@ -15195,7 +15195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="T68" sqref="T68"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added 2016 data. Interesting stuff.
</commit_message>
<xml_diff>
--- a/TJPW Metrics.xlsx
+++ b/TJPW Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3819" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3819" uniqueCount="805">
   <si>
     <t>`</t>
   </si>
@@ -1893,9 +1893,6 @@
     <t>Coconeri Hall</t>
   </si>
   <si>
-    <t>Maho vs Hinako</t>
-  </si>
-  <si>
     <t>KANNA vs Nodoka-Oneesan</t>
   </si>
   <si>
@@ -1920,9 +1917,6 @@
     <t>10m55s</t>
   </si>
   <si>
-    <t>Maho</t>
-  </si>
-  <si>
     <t>Hinako</t>
   </si>
   <si>
@@ -2437,6 +2431,9 @@
   </si>
   <si>
     <t>20m00s</t>
+  </si>
+  <si>
+    <t>Maho (Maho Kurone) vs Hinako</t>
   </si>
 </sst>
 </file>
@@ -14561,7 +14558,7 @@
         <v>52</v>
       </c>
       <c r="T33" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -14599,7 +14596,7 @@
         <v>52</v>
       </c>
       <c r="T34" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
@@ -14804,7 +14801,7 @@
         <v>52</v>
       </c>
       <c r="T39" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -14842,7 +14839,7 @@
         <v>52</v>
       </c>
       <c r="T40" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -16054,7 +16051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
@@ -17454,7 +17451,7 @@
         <v>52</v>
       </c>
       <c r="T35" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
@@ -17492,7 +17489,7 @@
         <v>52</v>
       </c>
       <c r="T36" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
@@ -17665,7 +17662,7 @@
         <v>52</v>
       </c>
       <c r="T40" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
@@ -17703,7 +17700,7 @@
         <v>52</v>
       </c>
       <c r="T41" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -19188,8 +19185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T142"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="H143" sqref="H143"/>
+    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21444,23 +21441,23 @@
         <v>209</v>
       </c>
       <c r="E55" t="s">
-        <v>624</v>
+        <v>804</v>
       </c>
       <c r="F55" s="60"/>
       <c r="H55" t="s">
-        <v>633</v>
+        <v>701</v>
       </c>
       <c r="I55" t="s">
         <v>51</v>
       </c>
       <c r="J55" t="s">
+        <v>632</v>
+      </c>
+      <c r="K55" t="s">
+        <v>52</v>
+      </c>
+      <c r="T55" t="s">
         <v>634</v>
-      </c>
-      <c r="K55" t="s">
-        <v>52</v>
-      </c>
-      <c r="T55" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
@@ -21477,10 +21474,10 @@
         <v>19</v>
       </c>
       <c r="E56" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F56" s="60" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G56" t="s">
         <v>149</v>
@@ -21512,10 +21509,10 @@
         <v>189</v>
       </c>
       <c r="E57" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F57" s="60" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G57" t="s">
         <v>149</v>
@@ -21553,16 +21550,16 @@
         <v>19</v>
       </c>
       <c r="E58" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F58" s="60" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G58" t="s">
         <v>155</v>
       </c>
       <c r="H58" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="I58" t="s">
         <v>51</v>
@@ -21588,10 +21585,10 @@
         <v>20</v>
       </c>
       <c r="E59" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F59" s="60" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G59" t="s">
         <v>149</v>
@@ -21623,13 +21620,13 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B60" s="61">
         <v>42539</v>
       </c>
       <c r="C60" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D60" t="s">
         <v>19</v>
@@ -21638,7 +21635,7 @@
         <v>618</v>
       </c>
       <c r="F60" s="60" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="G60" t="s">
         <v>149</v>
@@ -21658,13 +21655,13 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B61" s="61">
         <v>42539</v>
       </c>
       <c r="C61" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D61" t="s">
         <v>19</v>
@@ -21673,7 +21670,7 @@
         <v>577</v>
       </c>
       <c r="F61" s="60" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G61" t="s">
         <v>155</v>
@@ -21693,13 +21690,13 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B62" s="61">
         <v>42539</v>
       </c>
       <c r="C62" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D62" t="s">
         <v>19</v>
@@ -21708,7 +21705,7 @@
         <v>577</v>
       </c>
       <c r="F62" s="60" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="G62" t="s">
         <v>155</v>
@@ -21731,22 +21728,22 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B63" s="61">
         <v>42539</v>
       </c>
       <c r="C63" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D63" t="s">
         <v>20</v>
       </c>
       <c r="E63" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="F63" s="60" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="G63" t="s">
         <v>149</v>
@@ -21778,19 +21775,19 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B64" s="61">
         <v>42539</v>
       </c>
       <c r="C64" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D64" t="s">
         <v>19</v>
       </c>
       <c r="E64" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="F64" s="60" t="s">
         <v>499</v>
@@ -21813,22 +21810,22 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B65" s="61">
         <v>42539</v>
       </c>
       <c r="C65" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D65" t="s">
         <v>19</v>
       </c>
       <c r="E65" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F65" s="60" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G65" t="s">
         <v>149</v>
@@ -21848,22 +21845,22 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B66" s="61">
         <v>42539</v>
       </c>
       <c r="C66" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D66" t="s">
         <v>20</v>
       </c>
       <c r="E66" t="s">
+        <v>644</v>
+      </c>
+      <c r="F66" s="60" t="s">
         <v>646</v>
-      </c>
-      <c r="F66" s="60" t="s">
-        <v>648</v>
       </c>
       <c r="G66" t="s">
         <v>155</v>
@@ -21895,7 +21892,7 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B67" s="61">
         <v>42548</v>
@@ -21907,10 +21904,10 @@
         <v>19</v>
       </c>
       <c r="E67" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F67" s="60" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="G67" t="s">
         <v>155</v>
@@ -21930,7 +21927,7 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B68" s="61">
         <v>42548</v>
@@ -21942,7 +21939,7 @@
         <v>189</v>
       </c>
       <c r="E68" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F68" s="60" t="s">
         <v>369</v>
@@ -21971,7 +21968,7 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B69" s="61">
         <v>42548</v>
@@ -21983,7 +21980,7 @@
         <v>20</v>
       </c>
       <c r="E69" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="F69" s="60" t="s">
         <v>522</v>
@@ -22018,7 +22015,7 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B70" s="61">
         <v>42560</v>
@@ -22030,10 +22027,10 @@
         <v>19</v>
       </c>
       <c r="E70" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="F70" s="60" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="G70" t="s">
         <v>149</v>
@@ -22051,12 +22048,12 @@
         <v>52</v>
       </c>
       <c r="T70" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B71" s="61">
         <v>42560</v>
@@ -22089,12 +22086,12 @@
         <v>52</v>
       </c>
       <c r="T71" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B72" s="61">
         <v>42560</v>
@@ -22106,10 +22103,10 @@
         <v>20</v>
       </c>
       <c r="E72" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="F72" s="60" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="G72" t="s">
         <v>149</v>
@@ -22133,7 +22130,7 @@
         <v>175</v>
       </c>
       <c r="N72" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="O72" t="s">
         <v>52</v>
@@ -22141,7 +22138,7 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B73" s="61">
         <v>42560</v>
@@ -22153,10 +22150,10 @@
         <v>19</v>
       </c>
       <c r="E73" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F73" s="60" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="G73" t="s">
         <v>149</v>
@@ -22174,12 +22171,12 @@
         <v>52</v>
       </c>
       <c r="T73" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B74" s="61">
         <v>42560</v>
@@ -22191,10 +22188,10 @@
         <v>19</v>
       </c>
       <c r="E74" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F74" s="60" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="G74" t="s">
         <v>149</v>
@@ -22212,12 +22209,12 @@
         <v>52</v>
       </c>
       <c r="T74" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B75" s="61">
         <v>42574</v>
@@ -22232,7 +22229,7 @@
         <v>608</v>
       </c>
       <c r="F75" s="60" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G75" t="s">
         <v>155</v>
@@ -22250,12 +22247,12 @@
         <v>52</v>
       </c>
       <c r="T75" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B76" s="61">
         <v>42574</v>
@@ -22267,7 +22264,7 @@
         <v>19</v>
       </c>
       <c r="E76" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="F76" s="60" t="s">
         <v>279</v>
@@ -22288,12 +22285,12 @@
         <v>52</v>
       </c>
       <c r="T76" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B77" s="61">
         <v>42574</v>
@@ -22305,16 +22302,16 @@
         <v>19</v>
       </c>
       <c r="E77" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F77" s="60" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="G77" t="s">
         <v>155</v>
       </c>
       <c r="H77" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="I77" t="s">
         <v>51</v>
@@ -22328,7 +22325,7 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B78" s="61">
         <v>42574</v>
@@ -22340,10 +22337,10 @@
         <v>189</v>
       </c>
       <c r="E78" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F78" s="60" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="G78" t="s">
         <v>155</v>
@@ -22369,7 +22366,7 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B79" s="61">
         <v>42574</v>
@@ -22384,7 +22381,7 @@
         <v>600</v>
       </c>
       <c r="F79" s="60" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="G79" t="s">
         <v>149</v>
@@ -22402,12 +22399,12 @@
         <v>52</v>
       </c>
       <c r="T79" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B80" s="61">
         <v>42574</v>
@@ -22419,10 +22416,10 @@
         <v>19</v>
       </c>
       <c r="E80" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F80" s="60" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G80" t="s">
         <v>149</v>
@@ -22440,18 +22437,18 @@
         <v>52</v>
       </c>
       <c r="T80" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B81" s="61">
         <v>42581</v>
       </c>
       <c r="C81" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D81" t="s">
         <v>19</v>
@@ -22460,7 +22457,7 @@
         <v>598</v>
       </c>
       <c r="F81" s="60" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="G81" t="s">
         <v>149</v>
@@ -22480,22 +22477,22 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B82" s="61">
         <v>42581</v>
       </c>
       <c r="C82" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D82" t="s">
         <v>20</v>
       </c>
       <c r="E82" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="F82" s="60" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G82" t="s">
         <v>155</v>
@@ -22519,7 +22516,7 @@
         <v>175</v>
       </c>
       <c r="N82" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="O82" t="s">
         <v>52</v>
@@ -22527,13 +22524,13 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B83" s="61">
         <v>42581</v>
       </c>
       <c r="C83" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D83" t="s">
         <v>19</v>
@@ -22542,7 +22539,7 @@
         <v>424</v>
       </c>
       <c r="F83" s="60" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="G83" t="s">
         <v>149</v>
@@ -22562,22 +22559,22 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B84" s="61">
         <v>42581</v>
       </c>
       <c r="C84" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D84" t="s">
         <v>20</v>
       </c>
       <c r="E84" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F84" s="60" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="G84" t="s">
         <v>149</v>
@@ -22609,22 +22606,22 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B85" s="61">
         <v>42582</v>
       </c>
       <c r="C85" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D85" t="s">
         <v>19</v>
       </c>
       <c r="E85" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="F85" s="60" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G85" t="s">
         <v>155</v>
@@ -22644,22 +22641,22 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B86" s="61">
         <v>42582</v>
       </c>
       <c r="C86" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D86" t="s">
         <v>19</v>
       </c>
       <c r="E86" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="F86" s="60" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="G86" t="s">
         <v>149</v>
@@ -22679,22 +22676,22 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B87" s="61">
         <v>42582</v>
       </c>
       <c r="C87" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D87" t="s">
         <v>20</v>
       </c>
       <c r="E87" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="F87" s="60" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G87" t="s">
         <v>149</v>
@@ -22726,22 +22723,22 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B88" s="61">
         <v>42582</v>
       </c>
       <c r="C88" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="D88" t="s">
         <v>20</v>
       </c>
       <c r="E88" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F88" s="60" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G88" t="s">
         <v>149</v>
@@ -22773,7 +22770,7 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B89" s="61">
         <v>42595</v>
@@ -22785,7 +22782,7 @@
         <v>19</v>
       </c>
       <c r="E89" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="F89" s="60" t="s">
         <v>541</v>
@@ -22794,7 +22791,7 @@
         <v>149</v>
       </c>
       <c r="H89" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="I89" t="s">
         <v>51</v>
@@ -22808,7 +22805,7 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B90" s="61">
         <v>42595</v>
@@ -22823,7 +22820,7 @@
         <v>367</v>
       </c>
       <c r="F90" s="60" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G90" t="s">
         <v>149</v>
@@ -22841,12 +22838,12 @@
         <v>52</v>
       </c>
       <c r="T90" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B91" s="61">
         <v>42595</v>
@@ -22858,13 +22855,13 @@
         <v>19</v>
       </c>
       <c r="E91" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="F91" s="60" t="s">
         <v>308</v>
       </c>
       <c r="G91" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H91" t="s">
         <v>502</v>
@@ -22879,12 +22876,12 @@
         <v>52</v>
       </c>
       <c r="T91" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B92" s="61">
         <v>42595</v>
@@ -22896,10 +22893,10 @@
         <v>20</v>
       </c>
       <c r="E92" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="F92" s="60" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="G92" t="s">
         <v>149</v>
@@ -22929,12 +22926,12 @@
         <v>52</v>
       </c>
       <c r="T92" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B93" s="61">
         <v>42595</v>
@@ -22946,10 +22943,10 @@
         <v>20</v>
       </c>
       <c r="E93" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="F93" s="60" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G93" t="s">
         <v>149</v>
@@ -22973,7 +22970,7 @@
         <v>175</v>
       </c>
       <c r="N93" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="O93" t="s">
         <v>52</v>
@@ -22981,7 +22978,7 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B94" s="61">
         <v>42595</v>
@@ -22993,10 +22990,10 @@
         <v>19</v>
       </c>
       <c r="E94" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="F94" s="60" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G94" t="s">
         <v>155</v>
@@ -23014,12 +23011,12 @@
         <v>52</v>
       </c>
       <c r="T94" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B95" s="61">
         <v>42613</v>
@@ -23031,10 +23028,10 @@
         <v>189</v>
       </c>
       <c r="E95" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="F95" s="60" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="G95" t="s">
         <v>149</v>
@@ -23052,7 +23049,7 @@
         <v>175</v>
       </c>
       <c r="L95" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="M95" t="s">
         <v>52</v>
@@ -23060,7 +23057,7 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B96" s="61">
         <v>42613</v>
@@ -23072,7 +23069,7 @@
         <v>19</v>
       </c>
       <c r="E96" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F96" s="60" t="s">
         <v>308</v>
@@ -23081,7 +23078,7 @@
         <v>155</v>
       </c>
       <c r="H96" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="I96" t="s">
         <v>51</v>
@@ -23095,7 +23092,7 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B97" s="61">
         <v>42613</v>
@@ -23107,10 +23104,10 @@
         <v>19</v>
       </c>
       <c r="E97" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="F97" s="60" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G97" t="s">
         <v>149</v>
@@ -23130,7 +23127,7 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B98" s="61">
         <v>42613</v>
@@ -23142,10 +23139,10 @@
         <v>20</v>
       </c>
       <c r="E98" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="F98" s="60" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="G98" t="s">
         <v>155</v>
@@ -23177,7 +23174,7 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B99" s="61">
         <v>42613</v>
@@ -23192,7 +23189,7 @@
         <v>152</v>
       </c>
       <c r="F99" s="60" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G99" t="s">
         <v>149</v>
@@ -23212,22 +23209,22 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B100" s="61">
         <v>42630</v>
       </c>
       <c r="C100" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D100" t="s">
         <v>19</v>
       </c>
       <c r="E100" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="F100" s="60" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G100" t="s">
         <v>149</v>
@@ -23239,7 +23236,7 @@
         <v>51</v>
       </c>
       <c r="J100" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="K100" t="s">
         <v>52</v>
@@ -23247,19 +23244,19 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B101" s="61">
         <v>42630</v>
       </c>
       <c r="C101" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D101" t="s">
         <v>20</v>
       </c>
       <c r="E101" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="F101" s="60" t="s">
         <v>297</v>
@@ -23294,22 +23291,22 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B102" s="61">
         <v>42630</v>
       </c>
       <c r="C102" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D102" t="s">
         <v>189</v>
       </c>
       <c r="E102" t="s">
+        <v>719</v>
+      </c>
+      <c r="F102" s="60" t="s">
         <v>721</v>
-      </c>
-      <c r="F102" s="60" t="s">
-        <v>723</v>
       </c>
       <c r="G102" t="s">
         <v>149</v>
@@ -23335,13 +23332,13 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B103" s="61">
         <v>42630</v>
       </c>
       <c r="C103" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D103" t="s">
         <v>19</v>
@@ -23350,7 +23347,7 @@
         <v>598</v>
       </c>
       <c r="F103" s="60" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="G103" t="s">
         <v>149</v>
@@ -23370,13 +23367,13 @@
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B104" s="61">
         <v>42630</v>
       </c>
       <c r="C104" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D104" t="s">
         <v>20</v>
@@ -23385,7 +23382,7 @@
         <v>530</v>
       </c>
       <c r="F104" s="60" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="G104" t="s">
         <v>149</v>
@@ -23417,22 +23414,22 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B105" s="61">
         <v>42631</v>
       </c>
       <c r="C105" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D105" t="s">
         <v>20</v>
       </c>
       <c r="E105" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F105" s="60" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="G105" t="s">
         <v>149</v>
@@ -23464,19 +23461,19 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="B106" s="61">
         <v>42631</v>
       </c>
       <c r="C106" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D106" t="s">
         <v>19</v>
       </c>
       <c r="E106" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F106" s="60" t="s">
         <v>310</v>
@@ -23499,19 +23496,19 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B107" s="61">
         <v>42631</v>
       </c>
       <c r="C107" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D107" t="s">
         <v>19</v>
       </c>
       <c r="E107" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="F107" s="60" t="s">
         <v>369</v>
@@ -23526,7 +23523,7 @@
         <v>51</v>
       </c>
       <c r="J107" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="K107" t="s">
         <v>52</v>
@@ -23534,22 +23531,22 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B108" s="61">
         <v>42631</v>
       </c>
       <c r="C108" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D108" t="s">
         <v>19</v>
       </c>
       <c r="E108" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F108" s="60" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G108" t="s">
         <v>149</v>
@@ -23569,22 +23566,22 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B109" s="61">
         <v>42631</v>
       </c>
       <c r="C109" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D109" t="s">
         <v>20</v>
       </c>
       <c r="E109" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F109" s="60" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="G109" t="s">
         <v>149</v>
@@ -23616,7 +23613,7 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B110" s="61">
         <v>42635</v>
@@ -23628,10 +23625,10 @@
         <v>19</v>
       </c>
       <c r="E110" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="F110" s="60" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G110" t="s">
         <v>149</v>
@@ -23651,7 +23648,7 @@
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B111" s="61">
         <v>42635</v>
@@ -23663,7 +23660,7 @@
         <v>189</v>
       </c>
       <c r="E111" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F111" s="60" t="s">
         <v>585</v>
@@ -23692,7 +23689,7 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B112" s="61">
         <v>42635</v>
@@ -23704,10 +23701,10 @@
         <v>19</v>
       </c>
       <c r="E112" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="F112" s="60" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="G112" t="s">
         <v>149</v>
@@ -23727,7 +23724,7 @@
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B113" s="61">
         <v>42635</v>
@@ -23739,10 +23736,10 @@
         <v>423</v>
       </c>
       <c r="E113" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="F113" s="60" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="G113" t="s">
         <v>149</v>
@@ -23766,7 +23763,7 @@
         <v>51</v>
       </c>
       <c r="N113" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="O113" t="s">
         <v>175</v>
@@ -23784,12 +23781,12 @@
         <v>52</v>
       </c>
       <c r="T113" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B114" s="61">
         <v>42635</v>
@@ -23801,13 +23798,13 @@
         <v>19</v>
       </c>
       <c r="E114" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="F114" s="60" t="s">
         <v>562</v>
       </c>
       <c r="G114" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H114" t="s">
         <v>502</v>
@@ -23822,27 +23819,27 @@
         <v>52</v>
       </c>
       <c r="T114" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B115" s="61">
         <v>42659</v>
       </c>
       <c r="C115" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D115" t="s">
         <v>19</v>
       </c>
       <c r="E115" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="F115" s="60" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G115" t="s">
         <v>149</v>
@@ -23862,22 +23859,22 @@
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B116" s="61">
         <v>42659</v>
       </c>
       <c r="C116" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D116" t="s">
         <v>189</v>
       </c>
       <c r="E116" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="F116" s="60" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="G116" t="s">
         <v>149</v>
@@ -23895,7 +23892,7 @@
         <v>175</v>
       </c>
       <c r="L116" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="M116" t="s">
         <v>52</v>
@@ -23903,28 +23900,28 @@
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B117" s="61">
         <v>42659</v>
       </c>
       <c r="C117" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D117" t="s">
         <v>19</v>
       </c>
       <c r="E117" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="F117" s="60" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G117" t="s">
         <v>155</v>
       </c>
       <c r="H117" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="I117" t="s">
         <v>51</v>
@@ -23938,28 +23935,28 @@
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B118" s="61">
         <v>42659</v>
       </c>
       <c r="C118" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D118" t="s">
         <v>19</v>
       </c>
       <c r="E118" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F118" s="60" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="G118" t="s">
         <v>149</v>
       </c>
       <c r="H118" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="I118" t="s">
         <v>51</v>
@@ -23973,22 +23970,22 @@
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B119" s="61">
         <v>42659</v>
       </c>
       <c r="C119" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D119" t="s">
         <v>20</v>
       </c>
       <c r="E119" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F119" s="60" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G119" t="s">
         <v>149</v>
@@ -24020,22 +24017,22 @@
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B120" s="61">
         <v>42665</v>
       </c>
       <c r="C120" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D120" t="s">
         <v>19</v>
       </c>
       <c r="E120" t="s">
+        <v>761</v>
+      </c>
+      <c r="F120" s="60" t="s">
         <v>763</v>
-      </c>
-      <c r="F120" s="60" t="s">
-        <v>765</v>
       </c>
       <c r="G120" t="s">
         <v>149</v>
@@ -24047,7 +24044,7 @@
         <v>51</v>
       </c>
       <c r="J120" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="K120" t="s">
         <v>52</v>
@@ -24055,13 +24052,13 @@
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B121" s="61">
         <v>42665</v>
       </c>
       <c r="C121" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D121" t="s">
         <v>19</v>
@@ -24070,7 +24067,7 @@
         <v>537</v>
       </c>
       <c r="F121" s="60" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="G121" t="s">
         <v>149</v>
@@ -24090,22 +24087,22 @@
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B122" s="61">
         <v>42665</v>
       </c>
       <c r="C122" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D122" t="s">
         <v>20</v>
       </c>
       <c r="E122" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="F122" s="60" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="G122" t="s">
         <v>155</v>
@@ -24137,13 +24134,13 @@
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B123" s="61">
         <v>42665</v>
       </c>
       <c r="C123" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D123" t="s">
         <v>19</v>
@@ -24152,7 +24149,7 @@
         <v>462</v>
       </c>
       <c r="F123" s="60" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="G123" t="s">
         <v>149</v>
@@ -24172,19 +24169,19 @@
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B124" s="61">
         <v>42665</v>
       </c>
       <c r="C124" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D124" t="s">
         <v>19</v>
       </c>
       <c r="E124" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="F124" s="60" t="s">
         <v>330</v>
@@ -24193,7 +24190,7 @@
         <v>149</v>
       </c>
       <c r="H124" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="I124" t="s">
         <v>51</v>
@@ -24207,22 +24204,22 @@
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B125" s="61">
         <v>42665</v>
       </c>
       <c r="C125" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D125" t="s">
         <v>20</v>
       </c>
       <c r="E125" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="F125" s="60" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="G125" t="s">
         <v>149</v>
@@ -24254,7 +24251,7 @@
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B126" s="61">
         <v>42672</v>
@@ -24269,7 +24266,7 @@
         <v>462</v>
       </c>
       <c r="F126" s="60" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G126" t="s">
         <v>149</v>
@@ -24289,7 +24286,7 @@
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B127" s="61">
         <v>42672</v>
@@ -24301,16 +24298,16 @@
         <v>20</v>
       </c>
       <c r="E127" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="F127" s="60" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G127" t="s">
         <v>155</v>
       </c>
       <c r="H127" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="I127" t="s">
         <v>174</v>
@@ -24322,7 +24319,7 @@
         <v>51</v>
       </c>
       <c r="L127" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="M127" t="s">
         <v>175</v>
@@ -24336,7 +24333,7 @@
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B128" s="61">
         <v>42672</v>
@@ -24348,16 +24345,16 @@
         <v>189</v>
       </c>
       <c r="E128" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F128" s="60" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G128" t="s">
         <v>149</v>
       </c>
       <c r="H128" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="I128" t="s">
         <v>51</v>
@@ -24377,7 +24374,7 @@
     </row>
     <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B129" s="61">
         <v>42672</v>
@@ -24389,10 +24386,10 @@
         <v>19</v>
       </c>
       <c r="E129" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F129" s="60" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G129" t="s">
         <v>149</v>
@@ -24410,12 +24407,12 @@
         <v>52</v>
       </c>
       <c r="T129" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="B130" s="61">
         <v>42672</v>
@@ -24427,10 +24424,10 @@
         <v>19</v>
       </c>
       <c r="E130" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F130" s="60" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G130" t="s">
         <v>155</v>
@@ -24453,7 +24450,7 @@
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B131" s="61">
         <v>42686</v>
@@ -24465,10 +24462,10 @@
         <v>19</v>
       </c>
       <c r="E131" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="F131" s="60" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="G131" t="s">
         <v>155</v>
@@ -24488,7 +24485,7 @@
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B132" s="61">
         <v>42686</v>
@@ -24500,7 +24497,7 @@
         <v>20</v>
       </c>
       <c r="E132" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F132" s="60" t="s">
         <v>465</v>
@@ -24509,7 +24506,7 @@
         <v>149</v>
       </c>
       <c r="H132" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="I132" t="s">
         <v>174</v>
@@ -24535,7 +24532,7 @@
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B133" s="61">
         <v>42686</v>
@@ -24547,7 +24544,7 @@
         <v>19</v>
       </c>
       <c r="E133" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F133" s="60" t="s">
         <v>316</v>
@@ -24556,13 +24553,13 @@
         <v>149</v>
       </c>
       <c r="H133" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="I133" t="s">
         <v>51</v>
       </c>
       <c r="J133" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="K133" t="s">
         <v>52</v>
@@ -24570,7 +24567,7 @@
     </row>
     <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="B134" s="61">
         <v>42686</v>
@@ -24582,10 +24579,10 @@
         <v>20</v>
       </c>
       <c r="E134" t="s">
+        <v>781</v>
+      </c>
+      <c r="F134" s="60" t="s">
         <v>783</v>
-      </c>
-      <c r="F134" s="60" t="s">
-        <v>785</v>
       </c>
       <c r="G134" t="s">
         <v>149</v>
@@ -24617,7 +24614,7 @@
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B135" s="61">
         <v>42694</v>
@@ -24629,10 +24626,10 @@
         <v>19</v>
       </c>
       <c r="E135" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="F135" s="60" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="G135" t="s">
         <v>149</v>
@@ -24644,7 +24641,7 @@
         <v>51</v>
       </c>
       <c r="J135" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="K135" t="s">
         <v>52</v>
@@ -24652,7 +24649,7 @@
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B136" s="61">
         <v>42694</v>
@@ -24664,16 +24661,16 @@
         <v>20</v>
       </c>
       <c r="E136" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="F136" s="60" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="G136" t="s">
         <v>149</v>
       </c>
       <c r="H136" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="I136" t="s">
         <v>174</v>
@@ -24699,7 +24696,7 @@
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B137" s="61">
         <v>42694</v>
@@ -24711,7 +24708,7 @@
         <v>19</v>
       </c>
       <c r="E137" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="F137" s="60" t="s">
         <v>553</v>
@@ -24734,7 +24731,7 @@
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="B138" s="61">
         <v>42694</v>
@@ -24743,28 +24740,28 @@
         <v>527</v>
       </c>
       <c r="D138" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E138" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="F138" s="60" t="s">
         <v>459</v>
       </c>
       <c r="G138" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="H138" t="s">
         <v>101</v>
       </c>
       <c r="I138" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="J138" t="s">
         <v>214</v>
       </c>
       <c r="K138" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="L138" t="s">
         <v>144</v>
@@ -24773,12 +24770,12 @@
         <v>175</v>
       </c>
       <c r="T138" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B139" s="61">
         <v>42714</v>
@@ -24790,10 +24787,10 @@
         <v>19</v>
       </c>
       <c r="E139" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F139" s="60" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="G139" t="s">
         <v>149</v>
@@ -24813,7 +24810,7 @@
     </row>
     <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B140" s="61">
         <v>42714</v>
@@ -24825,10 +24822,10 @@
         <v>20</v>
       </c>
       <c r="E140" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="F140" s="60" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="G140" t="s">
         <v>155</v>
@@ -24860,7 +24857,7 @@
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B141" s="61">
         <v>42714</v>
@@ -24872,22 +24869,22 @@
         <v>19</v>
       </c>
       <c r="E141" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F141" s="60" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="G141" t="s">
         <v>155</v>
       </c>
       <c r="H141" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="I141" t="s">
         <v>51</v>
       </c>
       <c r="J141" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="K141" t="s">
         <v>52</v>
@@ -24895,7 +24892,7 @@
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B142" s="61">
         <v>42714</v>
@@ -24907,10 +24904,10 @@
         <v>20</v>
       </c>
       <c r="E142" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="F142" s="60" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G142" t="s">
         <v>159</v>
@@ -24934,7 +24931,7 @@
         <v>160</v>
       </c>
       <c r="N142" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="O142" t="s">
         <v>160</v>

</xml_diff>

<commit_message>
Added prior experience to spreadsheet
</commit_message>
<xml_diff>
--- a/TJPW Metrics.xlsx
+++ b/TJPW Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="2015 Matches" sheetId="5" r:id="rId4"/>
     <sheet name="2016 Matches" sheetId="6" r:id="rId5"/>
     <sheet name="2017 Matches" sheetId="7" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
+    <sheet name="Prior Experience" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5729" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5769" uniqueCount="1110">
   <si>
     <t>`</t>
   </si>
@@ -3341,6 +3341,15 @@
   </si>
   <si>
     <t>Christmas Special Big 5 Single Match</t>
+  </si>
+  <si>
+    <t>Wrestler</t>
+  </si>
+  <si>
+    <t>Matches</t>
+  </si>
+  <si>
+    <t>Years</t>
   </si>
 </sst>
 </file>
@@ -3897,6 +3906,66 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3998,66 +4067,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4452,97 +4461,97 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="68" t="s">
+      <c r="G2" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="87"/>
+      <c r="I2" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="71" t="s">
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="90"/>
+      <c r="M2" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="74" t="s">
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="77" t="s">
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="78"/>
-      <c r="AA2" s="78"/>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="79"/>
-      <c r="AG2" s="80" t="s">
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="98"/>
+      <c r="AC2" s="98"/>
+      <c r="AD2" s="98"/>
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="99"/>
+      <c r="AG2" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="AH2" s="81"/>
-      <c r="AI2" s="81"/>
-      <c r="AJ2" s="81"/>
-      <c r="AK2" s="81"/>
-      <c r="AL2" s="81"/>
-      <c r="AM2" s="81"/>
-      <c r="AN2" s="82"/>
-      <c r="AO2" s="83" t="s">
+      <c r="AH2" s="101"/>
+      <c r="AI2" s="101"/>
+      <c r="AJ2" s="101"/>
+      <c r="AK2" s="101"/>
+      <c r="AL2" s="101"/>
+      <c r="AM2" s="101"/>
+      <c r="AN2" s="102"/>
+      <c r="AO2" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="AP2" s="84"/>
-      <c r="AQ2" s="84"/>
-      <c r="AR2" s="84"/>
-      <c r="AS2" s="84"/>
-      <c r="AT2" s="85"/>
-      <c r="AU2" s="86" t="s">
+      <c r="AP2" s="104"/>
+      <c r="AQ2" s="104"/>
+      <c r="AR2" s="104"/>
+      <c r="AS2" s="104"/>
+      <c r="AT2" s="105"/>
+      <c r="AU2" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="AV2" s="87"/>
-      <c r="AW2" s="88" t="s">
+      <c r="AV2" s="107"/>
+      <c r="AW2" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="AX2" s="89"/>
-      <c r="AY2" s="89"/>
-      <c r="AZ2" s="89"/>
-      <c r="BA2" s="89"/>
-      <c r="BB2" s="89"/>
-      <c r="BC2" s="89"/>
-      <c r="BD2" s="90"/>
-      <c r="BE2" s="91" t="s">
+      <c r="AX2" s="109"/>
+      <c r="AY2" s="109"/>
+      <c r="AZ2" s="109"/>
+      <c r="BA2" s="109"/>
+      <c r="BB2" s="109"/>
+      <c r="BC2" s="109"/>
+      <c r="BD2" s="110"/>
+      <c r="BE2" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="BF2" s="92"/>
-      <c r="BG2" s="92"/>
-      <c r="BH2" s="93"/>
+      <c r="BF2" s="112"/>
+      <c r="BG2" s="112"/>
+      <c r="BH2" s="113"/>
       <c r="BI2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="BJ2" s="94" t="s">
+      <c r="BJ2" s="114" t="s">
         <v>12</v>
       </c>
-      <c r="BK2" s="95"/>
-      <c r="BL2" s="96"/>
-      <c r="BM2" s="63" t="s">
+      <c r="BK2" s="115"/>
+      <c r="BL2" s="116"/>
+      <c r="BM2" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="BN2" s="64"/>
-      <c r="BO2" s="64"/>
-      <c r="BP2" s="64"/>
-      <c r="BQ2" s="64"/>
-      <c r="BR2" s="64"/>
-      <c r="BS2" s="65"/>
+      <c r="BN2" s="84"/>
+      <c r="BO2" s="84"/>
+      <c r="BP2" s="84"/>
+      <c r="BQ2" s="84"/>
+      <c r="BR2" s="84"/>
+      <c r="BS2" s="85"/>
     </row>
     <row r="3" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
@@ -4563,18 +4572,18 @@
       <c r="F3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="99">
+      <c r="G3" s="74">
         <v>2020</v>
       </c>
-      <c r="H3" s="100"/>
-      <c r="I3" s="101" t="s">
+      <c r="H3" s="75"/>
+      <c r="I3" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="102"/>
-      <c r="K3" s="103" t="s">
+      <c r="J3" s="77"/>
+      <c r="K3" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="101"/>
+      <c r="L3" s="76"/>
       <c r="M3" s="14" t="s">
         <v>21</v>
       </c>
@@ -4605,74 +4614,74 @@
       <c r="V3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="W3" s="104" t="s">
+      <c r="W3" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="X3" s="105"/>
-      <c r="Y3" s="104" t="s">
+      <c r="X3" s="80"/>
+      <c r="Y3" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="Z3" s="106"/>
-      <c r="AA3" s="106" t="s">
+      <c r="Z3" s="81"/>
+      <c r="AA3" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="106"/>
-      <c r="AC3" s="106" t="s">
+      <c r="AB3" s="81"/>
+      <c r="AC3" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="AD3" s="106"/>
-      <c r="AE3" s="106" t="s">
+      <c r="AD3" s="81"/>
+      <c r="AE3" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="AF3" s="106"/>
-      <c r="AG3" s="97" t="s">
+      <c r="AF3" s="81"/>
+      <c r="AG3" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="98"/>
-      <c r="AI3" s="107" t="s">
+      <c r="AH3" s="73"/>
+      <c r="AI3" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="AJ3" s="97"/>
-      <c r="AK3" s="97" t="s">
+      <c r="AJ3" s="72"/>
+      <c r="AK3" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="AL3" s="97"/>
-      <c r="AM3" s="97" t="s">
+      <c r="AL3" s="72"/>
+      <c r="AM3" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="AN3" s="98"/>
-      <c r="AO3" s="111" t="s">
+      <c r="AN3" s="73"/>
+      <c r="AO3" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="AP3" s="112"/>
-      <c r="AQ3" s="111" t="s">
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="AR3" s="113"/>
-      <c r="AS3" s="113" t="s">
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="AT3" s="112"/>
-      <c r="AU3" s="114" t="s">
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="AV3" s="115"/>
-      <c r="AW3" s="116" t="s">
+      <c r="AV3" s="70"/>
+      <c r="AW3" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="AX3" s="108"/>
-      <c r="AY3" s="108" t="s">
+      <c r="AX3" s="63"/>
+      <c r="AY3" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="AZ3" s="108"/>
-      <c r="BA3" s="108" t="s">
+      <c r="AZ3" s="63"/>
+      <c r="BA3" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="BB3" s="108"/>
-      <c r="BC3" s="109" t="s">
+      <c r="BB3" s="63"/>
+      <c r="BC3" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="BD3" s="110"/>
+      <c r="BD3" s="65"/>
       <c r="BE3" s="22" t="s">
         <v>19</v>
       </c>
@@ -13563,14 +13572,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="BA3:BB3"/>
-    <mergeCell ref="BC3:BD3"/>
-    <mergeCell ref="AO3:AP3"/>
-    <mergeCell ref="AQ3:AR3"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AW3:AX3"/>
-    <mergeCell ref="AY3:AZ3"/>
+    <mergeCell ref="BM2:BS2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="W2:AF2"/>
+    <mergeCell ref="AG2:AN2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AW2:BD2"/>
+    <mergeCell ref="BE2:BH2"/>
+    <mergeCell ref="BJ2:BL2"/>
     <mergeCell ref="AM3:AN3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
@@ -13583,18 +13596,14 @@
     <mergeCell ref="AG3:AH3"/>
     <mergeCell ref="AI3:AJ3"/>
     <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="BM2:BS2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="M2:Q2"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="W2:AF2"/>
-    <mergeCell ref="AG2:AN2"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AW2:BD2"/>
-    <mergeCell ref="BE2:BH2"/>
-    <mergeCell ref="BJ2:BL2"/>
+    <mergeCell ref="BA3:BB3"/>
+    <mergeCell ref="BC3:BD3"/>
+    <mergeCell ref="AO3:AP3"/>
+    <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AY3:AZ3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25854,7 +25863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+    <sheetView topLeftCell="A143" workbookViewId="0">
       <selection activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
@@ -32412,14 +32421,436 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>170</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>420</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>362</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>363</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>460</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>475</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>502</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>503</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>524</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>525</v>
+      </c>
+      <c r="B22">
+        <v>304</v>
+      </c>
+      <c r="C22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>701</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>632</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>633</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>757</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>818</v>
+      </c>
+      <c r="B27">
+        <v>957</v>
+      </c>
+      <c r="C27">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>819</v>
+      </c>
+      <c r="B28">
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>820</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>827</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>828</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>873</v>
+      </c>
+      <c r="B32">
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>893</v>
+      </c>
+      <c r="B33">
+        <v>126</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>971</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>998</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>999</v>
+      </c>
+      <c r="B36">
+        <v>146</v>
+      </c>
+      <c r="C36">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B37">
+        <v>755</v>
+      </c>
+      <c r="C37">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B38">
+        <v>3283</v>
+      </c>
+      <c r="C38">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>